<commit_message>
All merges working. Staring to apply appropriate borders
</commit_message>
<xml_diff>
--- a/out.xlsx
+++ b/out.xlsx
@@ -28,15 +28,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0000FFFF"/>
+        <bgColor rgb="0000FFFF"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -44,13 +50,29 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="00000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="00000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="00000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="00000000"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -677,14 +699,135 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="n"/>
+      <c r="B1" s="2" t="n"/>
+      <c r="C1" s="2" t="n"/>
+      <c r="D1" s="2" t="n"/>
+      <c r="E1" s="2" t="n"/>
+      <c r="F1" s="2" t="n"/>
+      <c r="G1" s="2" t="n"/>
+      <c r="H1" s="2" t="n"/>
+      <c r="I1" s="2" t="n"/>
+      <c r="J1" s="2" t="n"/>
+      <c r="K1" s="2" t="n"/>
+      <c r="L1" s="2" t="n"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="n"/>
+      <c r="B2" s="2" t="n"/>
+      <c r="C2" s="2" t="n"/>
+      <c r="D2" s="2" t="n"/>
+      <c r="E2" s="2" t="n"/>
+      <c r="F2" s="2" t="n"/>
+      <c r="G2" s="2" t="n"/>
+      <c r="H2" s="2" t="n"/>
+      <c r="I2" s="2" t="n"/>
+      <c r="J2" s="2" t="n"/>
+      <c r="K2" s="2" t="n"/>
+      <c r="L2" s="2" t="n"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="n"/>
+      <c r="B3" s="3" t="n"/>
+      <c r="C3" s="3" t="n"/>
+      <c r="D3" s="3" t="n"/>
+      <c r="E3" s="3" t="n"/>
+      <c r="F3" s="3" t="n"/>
+      <c r="G3" s="3" t="n"/>
+      <c r="H3" s="3" t="n"/>
+      <c r="I3" s="3" t="n"/>
+      <c r="J3" s="3" t="n"/>
+      <c r="K3" s="3" t="n"/>
+      <c r="L3" s="3" t="n"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="n"/>
+      <c r="B4" s="3" t="n"/>
+      <c r="C4" s="3" t="n"/>
+      <c r="D4" s="3" t="n"/>
+      <c r="E4" s="3" t="n"/>
+      <c r="F4" s="3" t="n"/>
+      <c r="G4" s="3" t="n"/>
+      <c r="H4" s="3" t="n"/>
+      <c r="I4" s="3" t="n"/>
+      <c r="J4" s="3" t="n"/>
+      <c r="K4" s="3" t="n"/>
+      <c r="L4" s="3" t="n"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="n"/>
+      <c r="B5" s="3" t="n"/>
+      <c r="C5" s="3" t="n"/>
+      <c r="D5" s="3" t="n"/>
+      <c r="E5" s="3" t="n"/>
+      <c r="F5" s="3" t="n"/>
+      <c r="G5" s="3" t="n"/>
+      <c r="H5" s="3" t="n"/>
+      <c r="I5" s="3" t="n"/>
+      <c r="J5" s="3" t="n"/>
+      <c r="K5" s="3" t="n"/>
+      <c r="L5" s="3" t="n"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="3" t="n"/>
+      <c r="B6" s="3" t="n"/>
+      <c r="C6" s="3" t="n"/>
+      <c r="D6" s="3" t="n"/>
+      <c r="E6" s="3" t="n"/>
+      <c r="F6" s="3" t="n"/>
+      <c r="G6" s="3" t="n"/>
+      <c r="H6" s="3" t="n"/>
+      <c r="I6" s="3" t="n"/>
+      <c r="J6" s="3" t="n"/>
+      <c r="K6" s="3" t="n"/>
+      <c r="L6" s="3" t="n"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="3" t="n"/>
+      <c r="B7" s="3" t="n"/>
+      <c r="C7" s="3" t="n"/>
+      <c r="D7" s="3" t="n"/>
+      <c r="E7" s="3" t="n"/>
+      <c r="F7" s="3" t="n"/>
+      <c r="G7" s="3" t="n"/>
+      <c r="H7" s="3" t="n"/>
+      <c r="I7" s="3" t="n"/>
+      <c r="J7" s="3" t="n"/>
+      <c r="K7" s="3" t="n"/>
+      <c r="L7" s="3" t="n"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="3" t="n"/>
+      <c r="B8" s="3" t="n"/>
+      <c r="C8" s="3" t="n"/>
+      <c r="D8" s="3" t="n"/>
+      <c r="E8" s="3" t="n"/>
+      <c r="F8" s="3" t="n"/>
+      <c r="G8" s="3" t="n"/>
+      <c r="H8" s="3" t="n"/>
+      <c r="I8" s="3" t="n"/>
+      <c r="J8" s="3" t="n"/>
+      <c r="K8" s="3" t="n"/>
+      <c r="L8" s="3" t="n"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H2:L2"/>
+    <mergeCell ref="J3:L3"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Format all borders correctly.
</commit_message>
<xml_diff>
--- a/out.xlsx
+++ b/out.xlsx
@@ -42,7 +42,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -64,15 +64,113 @@
         <color rgb="00000000"/>
       </bottom>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="00000000"/>
+      </left>
+      <top style="medium">
+        <color rgb="00000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="00000000"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="medium">
+        <color rgb="00000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="00000000"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="medium">
+        <color rgb="00000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="00000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="00000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="00000000"/>
+      </left>
+      <top style="thin">
+        <color rgb="00000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="00000000"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin">
+        <color rgb="00000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="00000000"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="medium">
+        <color rgb="00000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="00000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="00000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="00000000"/>
+      </left>
+      <top style="thin">
+        <color rgb="00000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="00000000"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin">
+        <color rgb="00000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="00000000"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="medium">
+        <color rgb="00000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="00000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="00000000"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -737,87 +835,87 @@
     </row>
     <row r="3">
       <c r="A3" s="3" t="n"/>
-      <c r="B3" s="3" t="n"/>
-      <c r="C3" s="3" t="n"/>
+      <c r="B3" s="4" t="n"/>
+      <c r="C3" s="5" t="n"/>
       <c r="D3" s="3" t="n"/>
-      <c r="E3" s="3" t="n"/>
-      <c r="F3" s="3" t="n"/>
-      <c r="G3" s="3" t="n"/>
+      <c r="E3" s="4" t="n"/>
+      <c r="F3" s="4" t="n"/>
+      <c r="G3" s="5" t="n"/>
       <c r="H3" s="3" t="n"/>
-      <c r="I3" s="3" t="n"/>
-      <c r="J3" s="3" t="n"/>
-      <c r="K3" s="3" t="n"/>
-      <c r="L3" s="3" t="n"/>
+      <c r="I3" s="4" t="n"/>
+      <c r="J3" s="4" t="n"/>
+      <c r="K3" s="4" t="n"/>
+      <c r="L3" s="5" t="n"/>
     </row>
     <row r="4">
-      <c r="A4" s="3" t="n"/>
-      <c r="B4" s="3" t="n"/>
-      <c r="C4" s="3" t="n"/>
-      <c r="D4" s="3" t="n"/>
-      <c r="E4" s="3" t="n"/>
-      <c r="F4" s="3" t="n"/>
-      <c r="G4" s="3" t="n"/>
-      <c r="H4" s="3" t="n"/>
-      <c r="I4" s="3" t="n"/>
-      <c r="J4" s="3" t="n"/>
-      <c r="K4" s="3" t="n"/>
-      <c r="L4" s="3" t="n"/>
+      <c r="A4" s="6" t="n"/>
+      <c r="B4" s="7" t="n"/>
+      <c r="C4" s="8" t="n"/>
+      <c r="D4" s="6" t="n"/>
+      <c r="E4" s="7" t="n"/>
+      <c r="F4" s="7" t="n"/>
+      <c r="G4" s="8" t="n"/>
+      <c r="H4" s="6" t="n"/>
+      <c r="I4" s="7" t="n"/>
+      <c r="J4" s="7" t="n"/>
+      <c r="K4" s="7" t="n"/>
+      <c r="L4" s="8" t="n"/>
     </row>
     <row r="5">
-      <c r="A5" s="3" t="n"/>
-      <c r="B5" s="3" t="n"/>
-      <c r="C5" s="3" t="n"/>
-      <c r="D5" s="3" t="n"/>
-      <c r="E5" s="3" t="n"/>
-      <c r="F5" s="3" t="n"/>
-      <c r="G5" s="3" t="n"/>
-      <c r="H5" s="3" t="n"/>
-      <c r="I5" s="3" t="n"/>
-      <c r="J5" s="3" t="n"/>
-      <c r="K5" s="3" t="n"/>
-      <c r="L5" s="3" t="n"/>
+      <c r="A5" s="6" t="n"/>
+      <c r="B5" s="7" t="n"/>
+      <c r="C5" s="8" t="n"/>
+      <c r="D5" s="6" t="n"/>
+      <c r="E5" s="7" t="n"/>
+      <c r="F5" s="7" t="n"/>
+      <c r="G5" s="8" t="n"/>
+      <c r="H5" s="6" t="n"/>
+      <c r="I5" s="7" t="n"/>
+      <c r="J5" s="7" t="n"/>
+      <c r="K5" s="7" t="n"/>
+      <c r="L5" s="8" t="n"/>
     </row>
     <row r="6">
-      <c r="A6" s="3" t="n"/>
-      <c r="B6" s="3" t="n"/>
-      <c r="C6" s="3" t="n"/>
-      <c r="D6" s="3" t="n"/>
-      <c r="E6" s="3" t="n"/>
-      <c r="F6" s="3" t="n"/>
-      <c r="G6" s="3" t="n"/>
-      <c r="H6" s="3" t="n"/>
-      <c r="I6" s="3" t="n"/>
-      <c r="J6" s="3" t="n"/>
-      <c r="K6" s="3" t="n"/>
-      <c r="L6" s="3" t="n"/>
+      <c r="A6" s="6" t="n"/>
+      <c r="B6" s="7" t="n"/>
+      <c r="C6" s="8" t="n"/>
+      <c r="D6" s="6" t="n"/>
+      <c r="E6" s="7" t="n"/>
+      <c r="F6" s="7" t="n"/>
+      <c r="G6" s="8" t="n"/>
+      <c r="H6" s="6" t="n"/>
+      <c r="I6" s="7" t="n"/>
+      <c r="J6" s="7" t="n"/>
+      <c r="K6" s="7" t="n"/>
+      <c r="L6" s="8" t="n"/>
     </row>
     <row r="7">
-      <c r="A7" s="3" t="n"/>
-      <c r="B7" s="3" t="n"/>
-      <c r="C7" s="3" t="n"/>
-      <c r="D7" s="3" t="n"/>
-      <c r="E7" s="3" t="n"/>
-      <c r="F7" s="3" t="n"/>
-      <c r="G7" s="3" t="n"/>
-      <c r="H7" s="3" t="n"/>
-      <c r="I7" s="3" t="n"/>
-      <c r="J7" s="3" t="n"/>
-      <c r="K7" s="3" t="n"/>
-      <c r="L7" s="3" t="n"/>
+      <c r="A7" s="6" t="n"/>
+      <c r="B7" s="7" t="n"/>
+      <c r="C7" s="8" t="n"/>
+      <c r="D7" s="6" t="n"/>
+      <c r="E7" s="7" t="n"/>
+      <c r="F7" s="7" t="n"/>
+      <c r="G7" s="8" t="n"/>
+      <c r="H7" s="6" t="n"/>
+      <c r="I7" s="7" t="n"/>
+      <c r="J7" s="7" t="n"/>
+      <c r="K7" s="7" t="n"/>
+      <c r="L7" s="8" t="n"/>
     </row>
     <row r="8">
-      <c r="A8" s="3" t="n"/>
-      <c r="B8" s="3" t="n"/>
-      <c r="C8" s="3" t="n"/>
-      <c r="D8" s="3" t="n"/>
-      <c r="E8" s="3" t="n"/>
-      <c r="F8" s="3" t="n"/>
-      <c r="G8" s="3" t="n"/>
-      <c r="H8" s="3" t="n"/>
-      <c r="I8" s="3" t="n"/>
-      <c r="J8" s="3" t="n"/>
-      <c r="K8" s="3" t="n"/>
-      <c r="L8" s="3" t="n"/>
+      <c r="A8" s="9" t="n"/>
+      <c r="B8" s="10" t="n"/>
+      <c r="C8" s="11" t="n"/>
+      <c r="D8" s="9" t="n"/>
+      <c r="E8" s="10" t="n"/>
+      <c r="F8" s="10" t="n"/>
+      <c r="G8" s="11" t="n"/>
+      <c r="H8" s="9" t="n"/>
+      <c r="I8" s="10" t="n"/>
+      <c r="J8" s="10" t="n"/>
+      <c r="K8" s="10" t="n"/>
+      <c r="L8" s="11" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
Got Drivers Names being printed in correctly
</commit_message>
<xml_diff>
--- a/out.xlsx
+++ b/out.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-28920" yWindow="2445" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="19470" yWindow="2610" windowWidth="19080" windowHeight="15120" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="rawdata_Clio" sheetId="1" state="visible" r:id="rId1"/>
@@ -607,8 +607,8 @@
   </sheetPr>
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:H4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -724,23 +724,30 @@
       <c r="A4" t="n">
         <v>3</v>
       </c>
+      <c r="B4" s="1" t="n">
+        <v>44695</v>
+      </c>
       <c r="C4" t="n">
         <v>2</v>
       </c>
       <c r="D4" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E4" t="n">
         <v>1</v>
       </c>
       <c r="F4" t="n">
-        <v>3</v>
-      </c>
-      <c r="G4" t="n">
         <v>4</v>
       </c>
-      <c r="H4" t="n">
-        <v>6</v>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>DNP</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>DNP</t>
+        </is>
       </c>
     </row>
     <row r="5"/>
@@ -756,10 +763,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -867,6 +874,37 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="n">
+        <v>44696</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" t="n">
+        <v>2</v>
+      </c>
+      <c r="E4" t="n">
+        <v>3</v>
+      </c>
+      <c r="F4" t="n">
+        <v>4</v>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>DNP</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>DNP</t>
+        </is>
+      </c>
+    </row>
+    <row r="5"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -878,7 +916,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -981,75 +1019,162 @@
       <c r="L3" s="6" t="n"/>
     </row>
     <row r="4">
-      <c r="A4" s="7" t="n"/>
+      <c r="A4" s="7" t="inlineStr">
+        <is>
+          <t>Nathan</t>
+        </is>
+      </c>
       <c r="B4" s="8" t="n"/>
       <c r="C4" s="9" t="n"/>
-      <c r="D4" s="7" t="n"/>
+      <c r="D4" s="7" t="inlineStr">
+        <is>
+          <t>Nathan</t>
+        </is>
+      </c>
       <c r="E4" s="8" t="n"/>
       <c r="F4" s="8" t="n"/>
       <c r="G4" s="9" t="n"/>
-      <c r="H4" s="7" t="n"/>
+      <c r="H4" s="7" t="inlineStr">
+        <is>
+          <t>Nathan</t>
+        </is>
+      </c>
       <c r="I4" s="8" t="n"/>
       <c r="J4" s="8" t="n"/>
       <c r="K4" s="8" t="n"/>
       <c r="L4" s="9" t="n"/>
     </row>
     <row r="5">
-      <c r="A5" s="10" t="n"/>
+      <c r="A5" s="10" t="inlineStr">
+        <is>
+          <t>Evan</t>
+        </is>
+      </c>
       <c r="B5" s="8" t="n"/>
       <c r="C5" s="9" t="n"/>
-      <c r="D5" s="10" t="n"/>
+      <c r="D5" s="10" t="inlineStr">
+        <is>
+          <t>Evan</t>
+        </is>
+      </c>
       <c r="E5" s="8" t="n"/>
       <c r="F5" s="8" t="n"/>
       <c r="G5" s="9" t="n"/>
-      <c r="H5" s="10" t="n"/>
+      <c r="H5" s="10" t="inlineStr">
+        <is>
+          <t>Mike</t>
+        </is>
+      </c>
       <c r="I5" s="8" t="n"/>
       <c r="J5" s="8" t="n"/>
       <c r="K5" s="8" t="n"/>
       <c r="L5" s="9" t="n"/>
     </row>
     <row r="6">
-      <c r="A6" s="11" t="n"/>
+      <c r="A6" s="11" t="inlineStr">
+        <is>
+          <t>Mike</t>
+        </is>
+      </c>
       <c r="B6" s="8" t="n"/>
       <c r="C6" s="9" t="n"/>
-      <c r="D6" s="11" t="n"/>
+      <c r="D6" s="11" t="inlineStr">
+        <is>
+          <t>Mike</t>
+        </is>
+      </c>
       <c r="E6" s="8" t="n"/>
       <c r="F6" s="8" t="n"/>
       <c r="G6" s="9" t="n"/>
-      <c r="H6" s="11" t="n"/>
+      <c r="H6" s="11" t="inlineStr">
+        <is>
+          <t>Evan</t>
+        </is>
+      </c>
       <c r="I6" s="8" t="n"/>
       <c r="J6" s="8" t="n"/>
       <c r="K6" s="8" t="n"/>
       <c r="L6" s="9" t="n"/>
     </row>
     <row r="7">
-      <c r="A7" s="12" t="n"/>
+      <c r="A7" s="12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ray </t>
+        </is>
+      </c>
       <c r="B7" s="8" t="n"/>
       <c r="C7" s="9" t="n"/>
-      <c r="D7" s="12" t="n"/>
+      <c r="D7" s="12" t="inlineStr">
+        <is>
+          <t>Zach</t>
+        </is>
+      </c>
       <c r="E7" s="8" t="n"/>
       <c r="F7" s="8" t="n"/>
       <c r="G7" s="9" t="n"/>
-      <c r="H7" s="12" t="n"/>
+      <c r="H7" s="12" t="inlineStr">
+        <is>
+          <t>Zach</t>
+        </is>
+      </c>
       <c r="I7" s="8" t="n"/>
       <c r="J7" s="8" t="n"/>
       <c r="K7" s="8" t="n"/>
       <c r="L7" s="9" t="n"/>
     </row>
     <row r="8">
-      <c r="A8" s="13" t="n"/>
-      <c r="B8" s="14" t="n"/>
-      <c r="C8" s="15" t="n"/>
-      <c r="D8" s="13" t="n"/>
-      <c r="E8" s="14" t="n"/>
-      <c r="F8" s="14" t="n"/>
-      <c r="G8" s="15" t="n"/>
-      <c r="H8" s="13" t="n"/>
-      <c r="I8" s="14" t="n"/>
-      <c r="J8" s="14" t="n"/>
-      <c r="K8" s="14" t="n"/>
-      <c r="L8" s="15" t="n"/>
-    </row>
+      <c r="A8" s="12" t="inlineStr">
+        <is>
+          <t>Zach</t>
+        </is>
+      </c>
+      <c r="B8" s="8" t="n"/>
+      <c r="C8" s="9" t="n"/>
+      <c r="D8" s="12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ray </t>
+        </is>
+      </c>
+      <c r="E8" s="8" t="n"/>
+      <c r="F8" s="8" t="n"/>
+      <c r="G8" s="9" t="n"/>
+      <c r="H8" s="12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ray </t>
+        </is>
+      </c>
+      <c r="I8" s="8" t="n"/>
+      <c r="J8" s="8" t="n"/>
+      <c r="K8" s="8" t="n"/>
+      <c r="L8" s="9" t="n"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="13" t="inlineStr">
+        <is>
+          <t>Steve</t>
+        </is>
+      </c>
+      <c r="B9" s="14" t="n"/>
+      <c r="C9" s="15" t="n"/>
+      <c r="D9" s="13" t="inlineStr">
+        <is>
+          <t>Steve</t>
+        </is>
+      </c>
+      <c r="E9" s="14" t="n"/>
+      <c r="F9" s="14" t="n"/>
+      <c r="G9" s="15" t="n"/>
+      <c r="H9" s="13" t="inlineStr">
+        <is>
+          <t>Steve</t>
+        </is>
+      </c>
+      <c r="I9" s="14" t="n"/>
+      <c r="J9" s="14" t="n"/>
+      <c r="K9" s="14" t="n"/>
+      <c r="L9" s="15" t="n"/>
+    </row>
+    <row r="10"/>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="A1:L1"/>
@@ -1069,14 +1194,274 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>F3</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="n"/>
+      <c r="C1" s="2" t="n"/>
+      <c r="D1" s="2" t="n"/>
+      <c r="E1" s="2" t="n"/>
+      <c r="F1" s="2" t="n"/>
+      <c r="G1" s="2" t="n"/>
+      <c r="H1" s="2" t="n"/>
+      <c r="I1" s="2" t="n"/>
+      <c r="J1" s="2" t="n"/>
+      <c r="K1" s="2" t="n"/>
+      <c r="L1" s="2" t="n"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="3" t="inlineStr">
+        <is>
+          <t>Week 1</t>
+        </is>
+      </c>
+      <c r="B2" s="3" t="n"/>
+      <c r="C2" s="3" t="n"/>
+      <c r="D2" s="3" t="inlineStr">
+        <is>
+          <t>Week 2</t>
+        </is>
+      </c>
+      <c r="E2" s="3" t="n"/>
+      <c r="F2" s="3" t="n"/>
+      <c r="G2" s="3" t="n"/>
+      <c r="H2" s="3" t="inlineStr">
+        <is>
+          <t>Week 3</t>
+        </is>
+      </c>
+      <c r="I2" s="3" t="n"/>
+      <c r="J2" s="3" t="n"/>
+      <c r="K2" s="3" t="n"/>
+      <c r="L2" s="3" t="n"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="4" t="inlineStr">
+        <is>
+          <t>Driver</t>
+        </is>
+      </c>
+      <c r="B3" s="5" t="inlineStr">
+        <is>
+          <t>Pts</t>
+        </is>
+      </c>
+      <c r="C3" s="6" t="inlineStr">
+        <is>
+          <t>Finishes</t>
+        </is>
+      </c>
+      <c r="D3" s="4" t="inlineStr">
+        <is>
+          <t>Driver</t>
+        </is>
+      </c>
+      <c r="E3" s="5" t="inlineStr">
+        <is>
+          <t>Pts</t>
+        </is>
+      </c>
+      <c r="F3" s="5" t="inlineStr">
+        <is>
+          <t>Finishes</t>
+        </is>
+      </c>
+      <c r="G3" s="6" t="n"/>
+      <c r="H3" s="4" t="inlineStr">
+        <is>
+          <t>Driver</t>
+        </is>
+      </c>
+      <c r="I3" s="5" t="inlineStr">
+        <is>
+          <t>Pts</t>
+        </is>
+      </c>
+      <c r="J3" s="5" t="inlineStr">
+        <is>
+          <t>Finishes</t>
+        </is>
+      </c>
+      <c r="K3" s="5" t="n"/>
+      <c r="L3" s="6" t="n"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="7" t="inlineStr">
+        <is>
+          <t>Nathan</t>
+        </is>
+      </c>
+      <c r="B4" s="8" t="n"/>
+      <c r="C4" s="9" t="n"/>
+      <c r="D4" s="7" t="inlineStr">
+        <is>
+          <t>Evan</t>
+        </is>
+      </c>
+      <c r="E4" s="8" t="n"/>
+      <c r="F4" s="8" t="n"/>
+      <c r="G4" s="9" t="n"/>
+      <c r="H4" s="7" t="inlineStr">
+        <is>
+          <t>Nathan</t>
+        </is>
+      </c>
+      <c r="I4" s="8" t="n"/>
+      <c r="J4" s="8" t="n"/>
+      <c r="K4" s="8" t="n"/>
+      <c r="L4" s="9" t="n"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="10" t="inlineStr">
+        <is>
+          <t>Evan</t>
+        </is>
+      </c>
+      <c r="B5" s="8" t="n"/>
+      <c r="C5" s="9" t="n"/>
+      <c r="D5" s="10" t="inlineStr">
+        <is>
+          <t>Nathan</t>
+        </is>
+      </c>
+      <c r="E5" s="8" t="n"/>
+      <c r="F5" s="8" t="n"/>
+      <c r="G5" s="9" t="n"/>
+      <c r="H5" s="10" t="inlineStr">
+        <is>
+          <t>Evan</t>
+        </is>
+      </c>
+      <c r="I5" s="8" t="n"/>
+      <c r="J5" s="8" t="n"/>
+      <c r="K5" s="8" t="n"/>
+      <c r="L5" s="9" t="n"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ray </t>
+        </is>
+      </c>
+      <c r="B6" s="8" t="n"/>
+      <c r="C6" s="9" t="n"/>
+      <c r="D6" s="11" t="inlineStr">
+        <is>
+          <t>Mike</t>
+        </is>
+      </c>
+      <c r="E6" s="8" t="n"/>
+      <c r="F6" s="8" t="n"/>
+      <c r="G6" s="9" t="n"/>
+      <c r="H6" s="11" t="inlineStr">
+        <is>
+          <t>Mike</t>
+        </is>
+      </c>
+      <c r="I6" s="8" t="n"/>
+      <c r="J6" s="8" t="n"/>
+      <c r="K6" s="8" t="n"/>
+      <c r="L6" s="9" t="n"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="12" t="inlineStr">
+        <is>
+          <t>Mike</t>
+        </is>
+      </c>
+      <c r="B7" s="8" t="n"/>
+      <c r="C7" s="9" t="n"/>
+      <c r="D7" s="12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ray </t>
+        </is>
+      </c>
+      <c r="E7" s="8" t="n"/>
+      <c r="F7" s="8" t="n"/>
+      <c r="G7" s="9" t="n"/>
+      <c r="H7" s="12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ray </t>
+        </is>
+      </c>
+      <c r="I7" s="8" t="n"/>
+      <c r="J7" s="8" t="n"/>
+      <c r="K7" s="8" t="n"/>
+      <c r="L7" s="9" t="n"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="12" t="inlineStr">
+        <is>
+          <t>Zach</t>
+        </is>
+      </c>
+      <c r="B8" s="8" t="n"/>
+      <c r="C8" s="9" t="n"/>
+      <c r="D8" s="12" t="inlineStr">
+        <is>
+          <t>Zach</t>
+        </is>
+      </c>
+      <c r="E8" s="8" t="n"/>
+      <c r="F8" s="8" t="n"/>
+      <c r="G8" s="9" t="n"/>
+      <c r="H8" s="12" t="inlineStr">
+        <is>
+          <t>Zach</t>
+        </is>
+      </c>
+      <c r="I8" s="8" t="n"/>
+      <c r="J8" s="8" t="n"/>
+      <c r="K8" s="8" t="n"/>
+      <c r="L8" s="9" t="n"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="13" t="inlineStr">
+        <is>
+          <t>Steve</t>
+        </is>
+      </c>
+      <c r="B9" s="14" t="n"/>
+      <c r="C9" s="15" t="n"/>
+      <c r="D9" s="13" t="inlineStr">
+        <is>
+          <t>Steve</t>
+        </is>
+      </c>
+      <c r="E9" s="14" t="n"/>
+      <c r="F9" s="14" t="n"/>
+      <c r="G9" s="15" t="n"/>
+      <c r="H9" s="13" t="inlineStr">
+        <is>
+          <t>Steve</t>
+        </is>
+      </c>
+      <c r="I9" s="14" t="n"/>
+      <c r="J9" s="14" t="n"/>
+      <c r="K9" s="14" t="n"/>
+      <c r="L9" s="15" t="n"/>
+    </row>
+    <row r="10"/>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H2:L2"/>
+    <mergeCell ref="J3:L3"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Now Printing points with correct formatting. Switched background to white now.
</commit_message>
<xml_diff>
--- a/out.xlsx
+++ b/out.xlsx
@@ -19,7 +19,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="6">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -33,6 +33,18 @@
     </font>
     <font>
       <b val="1"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <color rgb="00FFD700"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <color rgb="00C0C0C0"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <color rgb="00CD7F32"/>
     </font>
   </fonts>
   <fills count="6">
@@ -183,7 +195,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -204,28 +216,43 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1024,155 +1051,191 @@
           <t>Nathan</t>
         </is>
       </c>
-      <c r="B4" s="8" t="n"/>
+      <c r="B4" s="8" t="n">
+        <v>25</v>
+      </c>
       <c r="C4" s="9" t="n"/>
       <c r="D4" s="7" t="inlineStr">
         <is>
           <t>Nathan</t>
         </is>
       </c>
-      <c r="E4" s="8" t="n"/>
-      <c r="F4" s="8" t="n"/>
+      <c r="E4" s="8" t="n">
+        <v>25</v>
+      </c>
+      <c r="F4" s="10" t="n"/>
       <c r="G4" s="9" t="n"/>
       <c r="H4" s="7" t="inlineStr">
         <is>
           <t>Nathan</t>
         </is>
       </c>
-      <c r="I4" s="8" t="n"/>
-      <c r="J4" s="8" t="n"/>
-      <c r="K4" s="8" t="n"/>
+      <c r="I4" s="8" t="n">
+        <v>25</v>
+      </c>
+      <c r="J4" s="10" t="n"/>
+      <c r="K4" s="10" t="n"/>
       <c r="L4" s="9" t="n"/>
     </row>
     <row r="5">
-      <c r="A5" s="10" t="inlineStr">
+      <c r="A5" s="11" t="inlineStr">
         <is>
           <t>Evan</t>
         </is>
       </c>
-      <c r="B5" s="8" t="n"/>
+      <c r="B5" s="12" t="n">
+        <v>18</v>
+      </c>
       <c r="C5" s="9" t="n"/>
-      <c r="D5" s="10" t="inlineStr">
+      <c r="D5" s="11" t="inlineStr">
         <is>
           <t>Evan</t>
         </is>
       </c>
-      <c r="E5" s="8" t="n"/>
-      <c r="F5" s="8" t="n"/>
+      <c r="E5" s="12" t="n">
+        <v>18</v>
+      </c>
+      <c r="F5" s="10" t="n"/>
       <c r="G5" s="9" t="n"/>
-      <c r="H5" s="10" t="inlineStr">
+      <c r="H5" s="11" t="inlineStr">
         <is>
           <t>Mike</t>
         </is>
       </c>
-      <c r="I5" s="8" t="n"/>
-      <c r="J5" s="8" t="n"/>
-      <c r="K5" s="8" t="n"/>
+      <c r="I5" s="12" t="n">
+        <v>25</v>
+      </c>
+      <c r="J5" s="10" t="n"/>
+      <c r="K5" s="10" t="n"/>
       <c r="L5" s="9" t="n"/>
     </row>
     <row r="6">
-      <c r="A6" s="11" t="inlineStr">
+      <c r="A6" s="13" t="inlineStr">
         <is>
           <t>Mike</t>
         </is>
       </c>
-      <c r="B6" s="8" t="n"/>
+      <c r="B6" s="14" t="n">
+        <v>15</v>
+      </c>
       <c r="C6" s="9" t="n"/>
-      <c r="D6" s="11" t="inlineStr">
+      <c r="D6" s="13" t="inlineStr">
         <is>
           <t>Mike</t>
         </is>
       </c>
-      <c r="E6" s="8" t="n"/>
-      <c r="F6" s="8" t="n"/>
+      <c r="E6" s="14" t="n">
+        <v>15</v>
+      </c>
+      <c r="F6" s="10" t="n"/>
       <c r="G6" s="9" t="n"/>
-      <c r="H6" s="11" t="inlineStr">
+      <c r="H6" s="13" t="inlineStr">
         <is>
           <t>Evan</t>
         </is>
       </c>
-      <c r="I6" s="8" t="n"/>
-      <c r="J6" s="8" t="n"/>
-      <c r="K6" s="8" t="n"/>
+      <c r="I6" s="14" t="n">
+        <v>18</v>
+      </c>
+      <c r="J6" s="10" t="n"/>
+      <c r="K6" s="10" t="n"/>
       <c r="L6" s="9" t="n"/>
     </row>
     <row r="7">
-      <c r="A7" s="12" t="inlineStr">
+      <c r="A7" s="15" t="inlineStr">
         <is>
           <t xml:space="preserve">Ray </t>
         </is>
       </c>
-      <c r="B7" s="8" t="n"/>
+      <c r="B7" s="16" t="n">
+        <v>12</v>
+      </c>
       <c r="C7" s="9" t="n"/>
-      <c r="D7" s="12" t="inlineStr">
+      <c r="D7" s="15" t="inlineStr">
         <is>
           <t>Zach</t>
         </is>
       </c>
-      <c r="E7" s="8" t="n"/>
-      <c r="F7" s="8" t="n"/>
+      <c r="E7" s="16" t="n">
+        <v>15</v>
+      </c>
+      <c r="F7" s="10" t="n"/>
       <c r="G7" s="9" t="n"/>
-      <c r="H7" s="12" t="inlineStr">
+      <c r="H7" s="15" t="inlineStr">
         <is>
           <t>Zach</t>
         </is>
       </c>
-      <c r="I7" s="8" t="n"/>
-      <c r="J7" s="8" t="n"/>
-      <c r="K7" s="8" t="n"/>
+      <c r="I7" s="16" t="n">
+        <v>15</v>
+      </c>
+      <c r="J7" s="10" t="n"/>
+      <c r="K7" s="10" t="n"/>
       <c r="L7" s="9" t="n"/>
     </row>
     <row r="8">
-      <c r="A8" s="12" t="inlineStr">
+      <c r="A8" s="15" t="inlineStr">
         <is>
           <t>Zach</t>
         </is>
       </c>
-      <c r="B8" s="8" t="n"/>
+      <c r="B8" s="16" t="n">
+        <v>0</v>
+      </c>
       <c r="C8" s="9" t="n"/>
-      <c r="D8" s="12" t="inlineStr">
+      <c r="D8" s="15" t="inlineStr">
         <is>
           <t xml:space="preserve">Ray </t>
         </is>
       </c>
-      <c r="E8" s="8" t="n"/>
-      <c r="F8" s="8" t="n"/>
+      <c r="E8" s="16" t="n">
+        <v>12</v>
+      </c>
+      <c r="F8" s="10" t="n"/>
       <c r="G8" s="9" t="n"/>
-      <c r="H8" s="12" t="inlineStr">
+      <c r="H8" s="15" t="inlineStr">
         <is>
           <t xml:space="preserve">Ray </t>
         </is>
       </c>
-      <c r="I8" s="8" t="n"/>
-      <c r="J8" s="8" t="n"/>
-      <c r="K8" s="8" t="n"/>
+      <c r="I8" s="16" t="n">
+        <v>12</v>
+      </c>
+      <c r="J8" s="10" t="n"/>
+      <c r="K8" s="10" t="n"/>
       <c r="L8" s="9" t="n"/>
     </row>
     <row r="9">
-      <c r="A9" s="13" t="inlineStr">
+      <c r="A9" s="17" t="inlineStr">
         <is>
           <t>Steve</t>
         </is>
       </c>
-      <c r="B9" s="14" t="n"/>
-      <c r="C9" s="15" t="n"/>
-      <c r="D9" s="13" t="inlineStr">
+      <c r="B9" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" s="19" t="n"/>
+      <c r="D9" s="17" t="inlineStr">
         <is>
           <t>Steve</t>
         </is>
       </c>
-      <c r="E9" s="14" t="n"/>
-      <c r="F9" s="14" t="n"/>
-      <c r="G9" s="15" t="n"/>
-      <c r="H9" s="13" t="inlineStr">
+      <c r="E9" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" s="20" t="n"/>
+      <c r="G9" s="19" t="n"/>
+      <c r="H9" s="17" t="inlineStr">
         <is>
           <t>Steve</t>
         </is>
       </c>
-      <c r="I9" s="14" t="n"/>
-      <c r="J9" s="14" t="n"/>
-      <c r="K9" s="14" t="n"/>
-      <c r="L9" s="15" t="n"/>
+      <c r="I9" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" s="20" t="n"/>
+      <c r="K9" s="20" t="n"/>
+      <c r="L9" s="19" t="n"/>
     </row>
     <row r="10"/>
   </sheetData>
@@ -1302,155 +1365,191 @@
           <t>Nathan</t>
         </is>
       </c>
-      <c r="B4" s="8" t="n"/>
+      <c r="B4" s="8" t="n">
+        <v>25</v>
+      </c>
       <c r="C4" s="9" t="n"/>
       <c r="D4" s="7" t="inlineStr">
         <is>
           <t>Evan</t>
         </is>
       </c>
-      <c r="E4" s="8" t="n"/>
-      <c r="F4" s="8" t="n"/>
+      <c r="E4" s="8" t="n">
+        <v>25</v>
+      </c>
+      <c r="F4" s="10" t="n"/>
       <c r="G4" s="9" t="n"/>
       <c r="H4" s="7" t="inlineStr">
         <is>
           <t>Nathan</t>
         </is>
       </c>
-      <c r="I4" s="8" t="n"/>
-      <c r="J4" s="8" t="n"/>
-      <c r="K4" s="8" t="n"/>
+      <c r="I4" s="8" t="n">
+        <v>25</v>
+      </c>
+      <c r="J4" s="10" t="n"/>
+      <c r="K4" s="10" t="n"/>
       <c r="L4" s="9" t="n"/>
     </row>
     <row r="5">
-      <c r="A5" s="10" t="inlineStr">
+      <c r="A5" s="11" t="inlineStr">
         <is>
           <t>Evan</t>
         </is>
       </c>
-      <c r="B5" s="8" t="n"/>
+      <c r="B5" s="12" t="n">
+        <v>18</v>
+      </c>
       <c r="C5" s="9" t="n"/>
-      <c r="D5" s="10" t="inlineStr">
+      <c r="D5" s="11" t="inlineStr">
         <is>
           <t>Nathan</t>
         </is>
       </c>
-      <c r="E5" s="8" t="n"/>
-      <c r="F5" s="8" t="n"/>
+      <c r="E5" s="12" t="n">
+        <v>25</v>
+      </c>
+      <c r="F5" s="10" t="n"/>
       <c r="G5" s="9" t="n"/>
-      <c r="H5" s="10" t="inlineStr">
+      <c r="H5" s="11" t="inlineStr">
         <is>
           <t>Evan</t>
         </is>
       </c>
-      <c r="I5" s="8" t="n"/>
-      <c r="J5" s="8" t="n"/>
-      <c r="K5" s="8" t="n"/>
+      <c r="I5" s="12" t="n">
+        <v>25</v>
+      </c>
+      <c r="J5" s="10" t="n"/>
+      <c r="K5" s="10" t="n"/>
       <c r="L5" s="9" t="n"/>
     </row>
     <row r="6">
-      <c r="A6" s="11" t="inlineStr">
+      <c r="A6" s="13" t="inlineStr">
         <is>
           <t xml:space="preserve">Ray </t>
         </is>
       </c>
-      <c r="B6" s="8" t="n"/>
+      <c r="B6" s="14" t="n">
+        <v>15</v>
+      </c>
       <c r="C6" s="9" t="n"/>
-      <c r="D6" s="11" t="inlineStr">
+      <c r="D6" s="13" t="inlineStr">
         <is>
           <t>Mike</t>
         </is>
       </c>
-      <c r="E6" s="8" t="n"/>
-      <c r="F6" s="8" t="n"/>
+      <c r="E6" s="14" t="n">
+        <v>18</v>
+      </c>
+      <c r="F6" s="10" t="n"/>
       <c r="G6" s="9" t="n"/>
-      <c r="H6" s="11" t="inlineStr">
+      <c r="H6" s="13" t="inlineStr">
         <is>
           <t>Mike</t>
         </is>
       </c>
-      <c r="I6" s="8" t="n"/>
-      <c r="J6" s="8" t="n"/>
-      <c r="K6" s="8" t="n"/>
+      <c r="I6" s="14" t="n">
+        <v>18</v>
+      </c>
+      <c r="J6" s="10" t="n"/>
+      <c r="K6" s="10" t="n"/>
       <c r="L6" s="9" t="n"/>
     </row>
     <row r="7">
-      <c r="A7" s="12" t="inlineStr">
+      <c r="A7" s="15" t="inlineStr">
         <is>
           <t>Mike</t>
         </is>
       </c>
-      <c r="B7" s="8" t="n"/>
+      <c r="B7" s="16" t="n">
+        <v>12</v>
+      </c>
       <c r="C7" s="9" t="n"/>
-      <c r="D7" s="12" t="inlineStr">
+      <c r="D7" s="15" t="inlineStr">
         <is>
           <t xml:space="preserve">Ray </t>
         </is>
       </c>
-      <c r="E7" s="8" t="n"/>
-      <c r="F7" s="8" t="n"/>
+      <c r="E7" s="16" t="n">
+        <v>15</v>
+      </c>
+      <c r="F7" s="10" t="n"/>
       <c r="G7" s="9" t="n"/>
-      <c r="H7" s="12" t="inlineStr">
+      <c r="H7" s="15" t="inlineStr">
         <is>
           <t xml:space="preserve">Ray </t>
         </is>
       </c>
-      <c r="I7" s="8" t="n"/>
-      <c r="J7" s="8" t="n"/>
-      <c r="K7" s="8" t="n"/>
+      <c r="I7" s="16" t="n">
+        <v>15</v>
+      </c>
+      <c r="J7" s="10" t="n"/>
+      <c r="K7" s="10" t="n"/>
       <c r="L7" s="9" t="n"/>
     </row>
     <row r="8">
-      <c r="A8" s="12" t="inlineStr">
+      <c r="A8" s="15" t="inlineStr">
         <is>
           <t>Zach</t>
         </is>
       </c>
-      <c r="B8" s="8" t="n"/>
+      <c r="B8" s="16" t="n">
+        <v>0</v>
+      </c>
       <c r="C8" s="9" t="n"/>
-      <c r="D8" s="12" t="inlineStr">
+      <c r="D8" s="15" t="inlineStr">
         <is>
           <t>Zach</t>
         </is>
       </c>
-      <c r="E8" s="8" t="n"/>
-      <c r="F8" s="8" t="n"/>
+      <c r="E8" s="16" t="n">
+        <v>15</v>
+      </c>
+      <c r="F8" s="10" t="n"/>
       <c r="G8" s="9" t="n"/>
-      <c r="H8" s="12" t="inlineStr">
+      <c r="H8" s="15" t="inlineStr">
         <is>
           <t>Zach</t>
         </is>
       </c>
-      <c r="I8" s="8" t="n"/>
-      <c r="J8" s="8" t="n"/>
-      <c r="K8" s="8" t="n"/>
+      <c r="I8" s="16" t="n">
+        <v>15</v>
+      </c>
+      <c r="J8" s="10" t="n"/>
+      <c r="K8" s="10" t="n"/>
       <c r="L8" s="9" t="n"/>
     </row>
     <row r="9">
-      <c r="A9" s="13" t="inlineStr">
+      <c r="A9" s="17" t="inlineStr">
         <is>
           <t>Steve</t>
         </is>
       </c>
-      <c r="B9" s="14" t="n"/>
-      <c r="C9" s="15" t="n"/>
-      <c r="D9" s="13" t="inlineStr">
+      <c r="B9" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" s="19" t="n"/>
+      <c r="D9" s="17" t="inlineStr">
         <is>
           <t>Steve</t>
         </is>
       </c>
-      <c r="E9" s="14" t="n"/>
-      <c r="F9" s="14" t="n"/>
-      <c r="G9" s="15" t="n"/>
-      <c r="H9" s="13" t="inlineStr">
+      <c r="E9" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" s="20" t="n"/>
+      <c r="G9" s="19" t="n"/>
+      <c r="H9" s="17" t="inlineStr">
         <is>
           <t>Steve</t>
         </is>
       </c>
-      <c r="I9" s="14" t="n"/>
-      <c r="J9" s="14" t="n"/>
-      <c r="K9" s="14" t="n"/>
-      <c r="L9" s="15" t="n"/>
+      <c r="I9" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" s="20" t="n"/>
+      <c r="K9" s="20" t="n"/>
+      <c r="L9" s="19" t="n"/>
     </row>
     <row r="10"/>
   </sheetData>

</xml_diff>

<commit_message>
Everything now working - Tweaked some styling
</commit_message>
<xml_diff>
--- a/out.xlsx
+++ b/out.xlsx
@@ -19,7 +19,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -36,15 +36,18 @@
     </font>
     <font>
       <b val="1"/>
-      <color rgb="00FFD700"/>
+      <color rgb="00ffc200"/>
     </font>
     <font>
       <b val="1"/>
-      <color rgb="00C0C0C0"/>
+      <color rgb="009a9a9a"/>
     </font>
     <font>
       <b val="1"/>
       <color rgb="00CD7F32"/>
+    </font>
+    <font>
+      <color rgb="00e6e6e6"/>
     </font>
   </fonts>
   <fills count="6">
@@ -56,8 +59,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="0000FFFF"/>
-        <bgColor rgb="0000FFFF"/>
+        <fgColor rgb="00FFFFFF"/>
+        <bgColor rgb="00FFFFFF"/>
       </patternFill>
     </fill>
     <fill>
@@ -195,7 +198,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -219,10 +222,13 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -231,28 +237,40 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -943,7 +961,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L10"/>
+  <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1054,7 +1072,11 @@
       <c r="B4" s="8" t="n">
         <v>25</v>
       </c>
-      <c r="C4" s="9" t="n"/>
+      <c r="C4" s="9" t="inlineStr">
+        <is>
+          <t>1st</t>
+        </is>
+      </c>
       <c r="D4" s="7" t="inlineStr">
         <is>
           <t>Nathan</t>
@@ -1063,8 +1085,16 @@
       <c r="E4" s="8" t="n">
         <v>25</v>
       </c>
-      <c r="F4" s="10" t="n"/>
-      <c r="G4" s="9" t="n"/>
+      <c r="F4" s="8" t="inlineStr">
+        <is>
+          <t>1st</t>
+        </is>
+      </c>
+      <c r="G4" s="10" t="inlineStr">
+        <is>
+          <t>1st</t>
+        </is>
+      </c>
       <c r="H4" s="7" t="inlineStr">
         <is>
           <t>Nathan</t>
@@ -1073,169 +1103,301 @@
       <c r="I4" s="8" t="n">
         <v>25</v>
       </c>
-      <c r="J4" s="10" t="n"/>
-      <c r="K4" s="10" t="n"/>
-      <c r="L4" s="9" t="n"/>
+      <c r="J4" s="8" t="inlineStr">
+        <is>
+          <t>1st</t>
+        </is>
+      </c>
+      <c r="K4" s="11" t="inlineStr">
+        <is>
+          <t>1st</t>
+        </is>
+      </c>
+      <c r="L4" s="10" t="inlineStr">
+        <is>
+          <t>2nd</t>
+        </is>
+      </c>
     </row>
     <row r="5">
-      <c r="A5" s="11" t="inlineStr">
+      <c r="A5" s="12" t="inlineStr">
         <is>
           <t>Evan</t>
         </is>
       </c>
-      <c r="B5" s="12" t="n">
+      <c r="B5" s="13" t="n">
         <v>18</v>
       </c>
-      <c r="C5" s="9" t="n"/>
-      <c r="D5" s="11" t="inlineStr">
+      <c r="C5" s="14" t="inlineStr">
+        <is>
+          <t>2nd</t>
+        </is>
+      </c>
+      <c r="D5" s="12" t="inlineStr">
         <is>
           <t>Evan</t>
         </is>
       </c>
-      <c r="E5" s="12" t="n">
+      <c r="E5" s="13" t="n">
         <v>18</v>
       </c>
-      <c r="F5" s="10" t="n"/>
-      <c r="G5" s="9" t="n"/>
-      <c r="H5" s="11" t="inlineStr">
+      <c r="F5" s="13" t="inlineStr">
+        <is>
+          <t>2nd</t>
+        </is>
+      </c>
+      <c r="G5" s="10" t="inlineStr">
+        <is>
+          <t>2nd</t>
+        </is>
+      </c>
+      <c r="H5" s="12" t="inlineStr">
         <is>
           <t>Mike</t>
         </is>
       </c>
-      <c r="I5" s="12" t="n">
+      <c r="I5" s="13" t="n">
         <v>25</v>
       </c>
-      <c r="J5" s="10" t="n"/>
-      <c r="K5" s="10" t="n"/>
-      <c r="L5" s="9" t="n"/>
+      <c r="J5" s="11" t="inlineStr">
+        <is>
+          <t>3rd</t>
+        </is>
+      </c>
+      <c r="K5" s="11" t="inlineStr">
+        <is>
+          <t>4th</t>
+        </is>
+      </c>
+      <c r="L5" s="9" t="inlineStr">
+        <is>
+          <t>1st</t>
+        </is>
+      </c>
     </row>
     <row r="6">
-      <c r="A6" s="13" t="inlineStr">
+      <c r="A6" s="15" t="inlineStr">
         <is>
           <t>Mike</t>
         </is>
       </c>
-      <c r="B6" s="14" t="n">
+      <c r="B6" s="16" t="n">
         <v>15</v>
       </c>
-      <c r="C6" s="9" t="n"/>
-      <c r="D6" s="13" t="inlineStr">
+      <c r="C6" s="17" t="inlineStr">
+        <is>
+          <t>3rd</t>
+        </is>
+      </c>
+      <c r="D6" s="15" t="inlineStr">
         <is>
           <t>Mike</t>
         </is>
       </c>
-      <c r="E6" s="14" t="n">
+      <c r="E6" s="16" t="n">
         <v>15</v>
       </c>
-      <c r="F6" s="10" t="n"/>
-      <c r="G6" s="9" t="n"/>
-      <c r="H6" s="13" t="inlineStr">
+      <c r="F6" s="16" t="inlineStr">
+        <is>
+          <t>3rd</t>
+        </is>
+      </c>
+      <c r="G6" s="10" t="inlineStr">
+        <is>
+          <t>4th</t>
+        </is>
+      </c>
+      <c r="H6" s="15" t="inlineStr">
         <is>
           <t>Evan</t>
         </is>
       </c>
-      <c r="I6" s="14" t="n">
+      <c r="I6" s="16" t="n">
         <v>18</v>
       </c>
-      <c r="J6" s="10" t="n"/>
-      <c r="K6" s="10" t="n"/>
-      <c r="L6" s="9" t="n"/>
+      <c r="J6" s="13" t="inlineStr">
+        <is>
+          <t>2nd</t>
+        </is>
+      </c>
+      <c r="K6" s="11" t="inlineStr">
+        <is>
+          <t>2nd</t>
+        </is>
+      </c>
+      <c r="L6" s="10" t="inlineStr">
+        <is>
+          <t>3rd</t>
+        </is>
+      </c>
     </row>
     <row r="7">
-      <c r="A7" s="15" t="inlineStr">
+      <c r="A7" s="18" t="inlineStr">
         <is>
           <t xml:space="preserve">Ray </t>
         </is>
       </c>
-      <c r="B7" s="16" t="n">
+      <c r="B7" s="19" t="n">
         <v>12</v>
       </c>
-      <c r="C7" s="9" t="n"/>
-      <c r="D7" s="15" t="inlineStr">
+      <c r="C7" s="20" t="inlineStr">
+        <is>
+          <t>4th</t>
+        </is>
+      </c>
+      <c r="D7" s="18" t="inlineStr">
         <is>
           <t>Zach</t>
         </is>
       </c>
-      <c r="E7" s="16" t="n">
+      <c r="E7" s="19" t="n">
         <v>15</v>
       </c>
-      <c r="F7" s="10" t="n"/>
-      <c r="G7" s="9" t="n"/>
-      <c r="H7" s="15" t="inlineStr">
+      <c r="F7" s="11" t="inlineStr">
+        <is>
+          <t>DNP</t>
+        </is>
+      </c>
+      <c r="G7" s="17" t="inlineStr">
+        <is>
+          <t>3rd</t>
+        </is>
+      </c>
+      <c r="H7" s="18" t="inlineStr">
         <is>
           <t>Zach</t>
         </is>
       </c>
-      <c r="I7" s="16" t="n">
+      <c r="I7" s="19" t="n">
         <v>15</v>
       </c>
-      <c r="J7" s="10" t="n"/>
-      <c r="K7" s="10" t="n"/>
-      <c r="L7" s="9" t="n"/>
+      <c r="J7" s="11" t="inlineStr">
+        <is>
+          <t>DNP</t>
+        </is>
+      </c>
+      <c r="K7" s="16" t="inlineStr">
+        <is>
+          <t>3rd</t>
+        </is>
+      </c>
+      <c r="L7" s="10" t="inlineStr">
+        <is>
+          <t>DNP</t>
+        </is>
+      </c>
     </row>
     <row r="8">
-      <c r="A8" s="15" t="inlineStr">
+      <c r="A8" s="18" t="inlineStr">
         <is>
           <t>Zach</t>
         </is>
       </c>
-      <c r="B8" s="16" t="n">
+      <c r="B8" s="19" t="n">
         <v>0</v>
       </c>
-      <c r="C8" s="9" t="n"/>
-      <c r="D8" s="15" t="inlineStr">
+      <c r="C8" s="20" t="inlineStr">
+        <is>
+          <t>DNP</t>
+        </is>
+      </c>
+      <c r="D8" s="18" t="inlineStr">
         <is>
           <t xml:space="preserve">Ray </t>
         </is>
       </c>
-      <c r="E8" s="16" t="n">
+      <c r="E8" s="19" t="n">
         <v>12</v>
       </c>
-      <c r="F8" s="10" t="n"/>
-      <c r="G8" s="9" t="n"/>
-      <c r="H8" s="15" t="inlineStr">
+      <c r="F8" s="19" t="inlineStr">
+        <is>
+          <t>4th</t>
+        </is>
+      </c>
+      <c r="G8" s="10" t="inlineStr">
+        <is>
+          <t>5th</t>
+        </is>
+      </c>
+      <c r="H8" s="18" t="inlineStr">
         <is>
           <t xml:space="preserve">Ray </t>
         </is>
       </c>
-      <c r="I8" s="16" t="n">
+      <c r="I8" s="19" t="n">
         <v>12</v>
       </c>
-      <c r="J8" s="10" t="n"/>
-      <c r="K8" s="10" t="n"/>
-      <c r="L8" s="9" t="n"/>
+      <c r="J8" s="19" t="inlineStr">
+        <is>
+          <t>4th</t>
+        </is>
+      </c>
+      <c r="K8" s="11" t="inlineStr">
+        <is>
+          <t>5th</t>
+        </is>
+      </c>
+      <c r="L8" s="10" t="inlineStr">
+        <is>
+          <t>4th</t>
+        </is>
+      </c>
     </row>
     <row r="9">
-      <c r="A9" s="17" t="inlineStr">
+      <c r="A9" s="21" t="inlineStr">
         <is>
           <t>Steve</t>
         </is>
       </c>
-      <c r="B9" s="18" t="n">
+      <c r="B9" s="22" t="n">
         <v>0</v>
       </c>
-      <c r="C9" s="19" t="n"/>
-      <c r="D9" s="17" t="inlineStr">
+      <c r="C9" s="23" t="inlineStr">
+        <is>
+          <t>DNP</t>
+        </is>
+      </c>
+      <c r="D9" s="21" t="inlineStr">
         <is>
           <t>Steve</t>
         </is>
       </c>
-      <c r="E9" s="18" t="n">
+      <c r="E9" s="22" t="n">
         <v>0</v>
       </c>
-      <c r="F9" s="20" t="n"/>
-      <c r="G9" s="19" t="n"/>
-      <c r="H9" s="17" t="inlineStr">
+      <c r="F9" s="22" t="inlineStr">
+        <is>
+          <t>DNP</t>
+        </is>
+      </c>
+      <c r="G9" s="24" t="inlineStr">
+        <is>
+          <t>DNP</t>
+        </is>
+      </c>
+      <c r="H9" s="21" t="inlineStr">
         <is>
           <t>Steve</t>
         </is>
       </c>
-      <c r="I9" s="18" t="n">
+      <c r="I9" s="22" t="n">
         <v>0</v>
       </c>
-      <c r="J9" s="20" t="n"/>
-      <c r="K9" s="20" t="n"/>
-      <c r="L9" s="19" t="n"/>
+      <c r="J9" s="22" t="inlineStr">
+        <is>
+          <t>DNP</t>
+        </is>
+      </c>
+      <c r="K9" s="25" t="inlineStr">
+        <is>
+          <t>DNP</t>
+        </is>
+      </c>
+      <c r="L9" s="24" t="inlineStr">
+        <is>
+          <t>DNP</t>
+        </is>
+      </c>
     </row>
     <row r="10"/>
   </sheetData>
@@ -1257,7 +1419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L10"/>
+  <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1368,7 +1530,11 @@
       <c r="B4" s="8" t="n">
         <v>25</v>
       </c>
-      <c r="C4" s="9" t="n"/>
+      <c r="C4" s="9" t="inlineStr">
+        <is>
+          <t>1st</t>
+        </is>
+      </c>
       <c r="D4" s="7" t="inlineStr">
         <is>
           <t>Evan</t>
@@ -1377,8 +1543,16 @@
       <c r="E4" s="8" t="n">
         <v>25</v>
       </c>
-      <c r="F4" s="10" t="n"/>
-      <c r="G4" s="9" t="n"/>
+      <c r="F4" s="11" t="inlineStr">
+        <is>
+          <t>2nd</t>
+        </is>
+      </c>
+      <c r="G4" s="9" t="inlineStr">
+        <is>
+          <t>1st</t>
+        </is>
+      </c>
       <c r="H4" s="7" t="inlineStr">
         <is>
           <t>Nathan</t>
@@ -1387,169 +1561,301 @@
       <c r="I4" s="8" t="n">
         <v>25</v>
       </c>
-      <c r="J4" s="10" t="n"/>
-      <c r="K4" s="10" t="n"/>
-      <c r="L4" s="9" t="n"/>
+      <c r="J4" s="8" t="inlineStr">
+        <is>
+          <t>1st</t>
+        </is>
+      </c>
+      <c r="K4" s="11" t="inlineStr">
+        <is>
+          <t>5th</t>
+        </is>
+      </c>
+      <c r="L4" s="10" t="inlineStr">
+        <is>
+          <t>1st</t>
+        </is>
+      </c>
     </row>
     <row r="5">
-      <c r="A5" s="11" t="inlineStr">
+      <c r="A5" s="12" t="inlineStr">
         <is>
           <t>Evan</t>
         </is>
       </c>
-      <c r="B5" s="12" t="n">
+      <c r="B5" s="13" t="n">
         <v>18</v>
       </c>
-      <c r="C5" s="9" t="n"/>
-      <c r="D5" s="11" t="inlineStr">
+      <c r="C5" s="14" t="inlineStr">
+        <is>
+          <t>2nd</t>
+        </is>
+      </c>
+      <c r="D5" s="12" t="inlineStr">
         <is>
           <t>Nathan</t>
         </is>
       </c>
-      <c r="E5" s="12" t="n">
+      <c r="E5" s="13" t="n">
         <v>25</v>
       </c>
-      <c r="F5" s="10" t="n"/>
-      <c r="G5" s="9" t="n"/>
-      <c r="H5" s="11" t="inlineStr">
+      <c r="F5" s="8" t="inlineStr">
+        <is>
+          <t>1st</t>
+        </is>
+      </c>
+      <c r="G5" s="10" t="inlineStr">
+        <is>
+          <t>5th</t>
+        </is>
+      </c>
+      <c r="H5" s="12" t="inlineStr">
         <is>
           <t>Evan</t>
         </is>
       </c>
-      <c r="I5" s="12" t="n">
+      <c r="I5" s="13" t="n">
         <v>25</v>
       </c>
-      <c r="J5" s="10" t="n"/>
-      <c r="K5" s="10" t="n"/>
-      <c r="L5" s="9" t="n"/>
+      <c r="J5" s="11" t="inlineStr">
+        <is>
+          <t>2nd</t>
+        </is>
+      </c>
+      <c r="K5" s="8" t="inlineStr">
+        <is>
+          <t>1st</t>
+        </is>
+      </c>
+      <c r="L5" s="10" t="inlineStr">
+        <is>
+          <t>2nd</t>
+        </is>
+      </c>
     </row>
     <row r="6">
-      <c r="A6" s="13" t="inlineStr">
+      <c r="A6" s="15" t="inlineStr">
         <is>
           <t xml:space="preserve">Ray </t>
         </is>
       </c>
-      <c r="B6" s="14" t="n">
+      <c r="B6" s="16" t="n">
         <v>15</v>
       </c>
-      <c r="C6" s="9" t="n"/>
-      <c r="D6" s="13" t="inlineStr">
+      <c r="C6" s="17" t="inlineStr">
+        <is>
+          <t>3rd</t>
+        </is>
+      </c>
+      <c r="D6" s="15" t="inlineStr">
         <is>
           <t>Mike</t>
         </is>
       </c>
-      <c r="E6" s="14" t="n">
+      <c r="E6" s="16" t="n">
         <v>18</v>
       </c>
-      <c r="F6" s="10" t="n"/>
-      <c r="G6" s="9" t="n"/>
-      <c r="H6" s="13" t="inlineStr">
+      <c r="F6" s="11" t="inlineStr">
+        <is>
+          <t>4th</t>
+        </is>
+      </c>
+      <c r="G6" s="14" t="inlineStr">
+        <is>
+          <t>2nd</t>
+        </is>
+      </c>
+      <c r="H6" s="15" t="inlineStr">
         <is>
           <t>Mike</t>
         </is>
       </c>
-      <c r="I6" s="14" t="n">
+      <c r="I6" s="16" t="n">
         <v>18</v>
       </c>
-      <c r="J6" s="10" t="n"/>
-      <c r="K6" s="10" t="n"/>
-      <c r="L6" s="9" t="n"/>
+      <c r="J6" s="11" t="inlineStr">
+        <is>
+          <t>4th</t>
+        </is>
+      </c>
+      <c r="K6" s="13" t="inlineStr">
+        <is>
+          <t>2nd</t>
+        </is>
+      </c>
+      <c r="L6" s="10" t="inlineStr">
+        <is>
+          <t>3rd</t>
+        </is>
+      </c>
     </row>
     <row r="7">
-      <c r="A7" s="15" t="inlineStr">
+      <c r="A7" s="18" t="inlineStr">
         <is>
           <t>Mike</t>
         </is>
       </c>
-      <c r="B7" s="16" t="n">
+      <c r="B7" s="19" t="n">
         <v>12</v>
       </c>
-      <c r="C7" s="9" t="n"/>
-      <c r="D7" s="15" t="inlineStr">
+      <c r="C7" s="20" t="inlineStr">
+        <is>
+          <t>4th</t>
+        </is>
+      </c>
+      <c r="D7" s="18" t="inlineStr">
         <is>
           <t xml:space="preserve">Ray </t>
         </is>
       </c>
-      <c r="E7" s="16" t="n">
+      <c r="E7" s="19" t="n">
         <v>15</v>
       </c>
-      <c r="F7" s="10" t="n"/>
-      <c r="G7" s="9" t="n"/>
-      <c r="H7" s="15" t="inlineStr">
+      <c r="F7" s="16" t="inlineStr">
+        <is>
+          <t>3rd</t>
+        </is>
+      </c>
+      <c r="G7" s="10" t="inlineStr">
+        <is>
+          <t>4th</t>
+        </is>
+      </c>
+      <c r="H7" s="18" t="inlineStr">
         <is>
           <t xml:space="preserve">Ray </t>
         </is>
       </c>
-      <c r="I7" s="16" t="n">
+      <c r="I7" s="19" t="n">
         <v>15</v>
       </c>
-      <c r="J7" s="10" t="n"/>
-      <c r="K7" s="10" t="n"/>
-      <c r="L7" s="9" t="n"/>
+      <c r="J7" s="16" t="inlineStr">
+        <is>
+          <t>3rd</t>
+        </is>
+      </c>
+      <c r="K7" s="11" t="inlineStr">
+        <is>
+          <t>4th</t>
+        </is>
+      </c>
+      <c r="L7" s="10" t="inlineStr">
+        <is>
+          <t>4th</t>
+        </is>
+      </c>
     </row>
     <row r="8">
-      <c r="A8" s="15" t="inlineStr">
+      <c r="A8" s="18" t="inlineStr">
         <is>
           <t>Zach</t>
         </is>
       </c>
-      <c r="B8" s="16" t="n">
+      <c r="B8" s="19" t="n">
         <v>0</v>
       </c>
-      <c r="C8" s="9" t="n"/>
-      <c r="D8" s="15" t="inlineStr">
+      <c r="C8" s="20" t="inlineStr">
+        <is>
+          <t>DNP</t>
+        </is>
+      </c>
+      <c r="D8" s="18" t="inlineStr">
         <is>
           <t>Zach</t>
         </is>
       </c>
-      <c r="E8" s="16" t="n">
+      <c r="E8" s="19" t="n">
         <v>15</v>
       </c>
-      <c r="F8" s="10" t="n"/>
-      <c r="G8" s="9" t="n"/>
-      <c r="H8" s="15" t="inlineStr">
+      <c r="F8" s="11" t="inlineStr">
+        <is>
+          <t>DNP</t>
+        </is>
+      </c>
+      <c r="G8" s="17" t="inlineStr">
+        <is>
+          <t>3rd</t>
+        </is>
+      </c>
+      <c r="H8" s="18" t="inlineStr">
         <is>
           <t>Zach</t>
         </is>
       </c>
-      <c r="I8" s="16" t="n">
+      <c r="I8" s="19" t="n">
         <v>15</v>
       </c>
-      <c r="J8" s="10" t="n"/>
-      <c r="K8" s="10" t="n"/>
-      <c r="L8" s="9" t="n"/>
+      <c r="J8" s="11" t="inlineStr">
+        <is>
+          <t>DNP</t>
+        </is>
+      </c>
+      <c r="K8" s="16" t="inlineStr">
+        <is>
+          <t>3rd</t>
+        </is>
+      </c>
+      <c r="L8" s="10" t="inlineStr">
+        <is>
+          <t>DNP</t>
+        </is>
+      </c>
     </row>
     <row r="9">
-      <c r="A9" s="17" t="inlineStr">
+      <c r="A9" s="21" t="inlineStr">
         <is>
           <t>Steve</t>
         </is>
       </c>
-      <c r="B9" s="18" t="n">
+      <c r="B9" s="22" t="n">
         <v>0</v>
       </c>
-      <c r="C9" s="19" t="n"/>
-      <c r="D9" s="17" t="inlineStr">
+      <c r="C9" s="23" t="inlineStr">
+        <is>
+          <t>DNP</t>
+        </is>
+      </c>
+      <c r="D9" s="21" t="inlineStr">
         <is>
           <t>Steve</t>
         </is>
       </c>
-      <c r="E9" s="18" t="n">
+      <c r="E9" s="22" t="n">
         <v>0</v>
       </c>
-      <c r="F9" s="20" t="n"/>
-      <c r="G9" s="19" t="n"/>
-      <c r="H9" s="17" t="inlineStr">
+      <c r="F9" s="22" t="inlineStr">
+        <is>
+          <t>DNP</t>
+        </is>
+      </c>
+      <c r="G9" s="24" t="inlineStr">
+        <is>
+          <t>DNP</t>
+        </is>
+      </c>
+      <c r="H9" s="21" t="inlineStr">
         <is>
           <t>Steve</t>
         </is>
       </c>
-      <c r="I9" s="18" t="n">
+      <c r="I9" s="22" t="n">
         <v>0</v>
       </c>
-      <c r="J9" s="20" t="n"/>
-      <c r="K9" s="20" t="n"/>
-      <c r="L9" s="19" t="n"/>
+      <c r="J9" s="22" t="inlineStr">
+        <is>
+          <t>DNP</t>
+        </is>
+      </c>
+      <c r="K9" s="25" t="inlineStr">
+        <is>
+          <t>DNP</t>
+        </is>
+      </c>
+      <c r="L9" s="24" t="inlineStr">
+        <is>
+          <t>DNP</t>
+        </is>
+      </c>
     </row>
     <row r="10"/>
   </sheetData>

</xml_diff>

<commit_message>
Made DropWeeks a global var type declaration up top.
</commit_message>
<xml_diff>
--- a/out.xlsx
+++ b/out.xlsx
@@ -19,7 +19,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -45,9 +45,6 @@
     <font>
       <b val="1"/>
       <color rgb="00CD7F32"/>
-    </font>
-    <font>
-      <color rgb="00e6e6e6"/>
     </font>
   </fonts>
   <fills count="6">
@@ -198,7 +195,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -225,10 +222,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -237,27 +231,24 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -265,12 +256,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1083,14 +1068,14 @@
         </is>
       </c>
       <c r="E4" s="8" t="n">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="F4" s="8" t="inlineStr">
         <is>
           <t>1st</t>
         </is>
       </c>
-      <c r="G4" s="10" t="inlineStr">
+      <c r="G4" s="9" t="inlineStr">
         <is>
           <t>1st</t>
         </is>
@@ -1101,14 +1086,14 @@
         </is>
       </c>
       <c r="I4" s="8" t="n">
-        <v>25</v>
+        <v>68</v>
       </c>
       <c r="J4" s="8" t="inlineStr">
         <is>
           <t>1st</t>
         </is>
       </c>
-      <c r="K4" s="11" t="inlineStr">
+      <c r="K4" s="8" t="inlineStr">
         <is>
           <t>1st</t>
         </is>
@@ -1120,28 +1105,28 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="12" t="inlineStr">
+      <c r="A5" s="11" t="inlineStr">
         <is>
           <t>Evan</t>
         </is>
       </c>
-      <c r="B5" s="13" t="n">
+      <c r="B5" s="12" t="n">
         <v>18</v>
       </c>
-      <c r="C5" s="14" t="inlineStr">
+      <c r="C5" s="10" t="inlineStr">
         <is>
           <t>2nd</t>
         </is>
       </c>
-      <c r="D5" s="12" t="inlineStr">
+      <c r="D5" s="11" t="inlineStr">
         <is>
           <t>Evan</t>
         </is>
       </c>
-      <c r="E5" s="13" t="n">
-        <v>18</v>
-      </c>
-      <c r="F5" s="13" t="inlineStr">
+      <c r="E5" s="12" t="n">
+        <v>36</v>
+      </c>
+      <c r="F5" s="12" t="inlineStr">
         <is>
           <t>2nd</t>
         </is>
@@ -1151,20 +1136,20 @@
           <t>2nd</t>
         </is>
       </c>
-      <c r="H5" s="12" t="inlineStr">
+      <c r="H5" s="11" t="inlineStr">
         <is>
           <t>Mike</t>
         </is>
       </c>
-      <c r="I5" s="13" t="n">
-        <v>25</v>
-      </c>
-      <c r="J5" s="11" t="inlineStr">
+      <c r="I5" s="12" t="n">
+        <v>52</v>
+      </c>
+      <c r="J5" s="13" t="inlineStr">
         <is>
           <t>3rd</t>
         </is>
       </c>
-      <c r="K5" s="11" t="inlineStr">
+      <c r="K5" s="14" t="inlineStr">
         <is>
           <t>4th</t>
         </is>
@@ -1181,10 +1166,10 @@
           <t>Mike</t>
         </is>
       </c>
-      <c r="B6" s="16" t="n">
+      <c r="B6" s="13" t="n">
         <v>15</v>
       </c>
-      <c r="C6" s="17" t="inlineStr">
+      <c r="C6" s="16" t="inlineStr">
         <is>
           <t>3rd</t>
         </is>
@@ -1194,15 +1179,15 @@
           <t>Mike</t>
         </is>
       </c>
-      <c r="E6" s="16" t="n">
-        <v>15</v>
-      </c>
-      <c r="F6" s="16" t="inlineStr">
+      <c r="E6" s="13" t="n">
+        <v>27</v>
+      </c>
+      <c r="F6" s="13" t="inlineStr">
         <is>
           <t>3rd</t>
         </is>
       </c>
-      <c r="G6" s="10" t="inlineStr">
+      <c r="G6" s="17" t="inlineStr">
         <is>
           <t>4th</t>
         </is>
@@ -1212,20 +1197,20 @@
           <t>Evan</t>
         </is>
       </c>
-      <c r="I6" s="16" t="n">
-        <v>18</v>
-      </c>
-      <c r="J6" s="13" t="inlineStr">
+      <c r="I6" s="13" t="n">
+        <v>51</v>
+      </c>
+      <c r="J6" s="12" t="inlineStr">
         <is>
           <t>2nd</t>
         </is>
       </c>
-      <c r="K6" s="11" t="inlineStr">
+      <c r="K6" s="12" t="inlineStr">
         <is>
           <t>2nd</t>
         </is>
       </c>
-      <c r="L6" s="10" t="inlineStr">
+      <c r="L6" s="16" t="inlineStr">
         <is>
           <t>3rd</t>
         </is>
@@ -1237,53 +1222,53 @@
           <t xml:space="preserve">Ray </t>
         </is>
       </c>
-      <c r="B7" s="19" t="n">
+      <c r="B7" s="14" t="n">
         <v>12</v>
       </c>
-      <c r="C7" s="20" t="inlineStr">
+      <c r="C7" s="17" t="inlineStr">
         <is>
           <t>4th</t>
         </is>
       </c>
       <c r="D7" s="18" t="inlineStr">
         <is>
-          <t>Zach</t>
-        </is>
-      </c>
-      <c r="E7" s="19" t="n">
-        <v>15</v>
-      </c>
-      <c r="F7" s="11" t="inlineStr">
-        <is>
-          <t>DNP</t>
+          <t xml:space="preserve">Ray </t>
+        </is>
+      </c>
+      <c r="E7" s="14" t="n">
+        <v>22</v>
+      </c>
+      <c r="F7" s="14" t="inlineStr">
+        <is>
+          <t>4th</t>
         </is>
       </c>
       <c r="G7" s="17" t="inlineStr">
         <is>
-          <t>3rd</t>
+          <t>5th</t>
         </is>
       </c>
       <c r="H7" s="18" t="inlineStr">
         <is>
-          <t>Zach</t>
-        </is>
-      </c>
-      <c r="I7" s="19" t="n">
-        <v>15</v>
-      </c>
-      <c r="J7" s="11" t="inlineStr">
-        <is>
-          <t>DNP</t>
-        </is>
-      </c>
-      <c r="K7" s="16" t="inlineStr">
-        <is>
-          <t>3rd</t>
-        </is>
-      </c>
-      <c r="L7" s="10" t="inlineStr">
-        <is>
-          <t>DNP</t>
+          <t xml:space="preserve">Ray </t>
+        </is>
+      </c>
+      <c r="I7" s="14" t="n">
+        <v>34</v>
+      </c>
+      <c r="J7" s="14" t="inlineStr">
+        <is>
+          <t>4th</t>
+        </is>
+      </c>
+      <c r="K7" s="14" t="inlineStr">
+        <is>
+          <t>5th</t>
+        </is>
+      </c>
+      <c r="L7" s="17" t="inlineStr">
+        <is>
+          <t>4th</t>
         </is>
       </c>
     </row>
@@ -1293,107 +1278,107 @@
           <t>Zach</t>
         </is>
       </c>
-      <c r="B8" s="19" t="n">
+      <c r="B8" s="14" t="n">
         <v>0</v>
       </c>
-      <c r="C8" s="20" t="inlineStr">
+      <c r="C8" s="17" t="inlineStr">
         <is>
           <t>DNP</t>
         </is>
       </c>
       <c r="D8" s="18" t="inlineStr">
         <is>
-          <t xml:space="preserve">Ray </t>
-        </is>
-      </c>
-      <c r="E8" s="19" t="n">
-        <v>12</v>
-      </c>
-      <c r="F8" s="19" t="inlineStr">
-        <is>
-          <t>4th</t>
-        </is>
-      </c>
-      <c r="G8" s="10" t="inlineStr">
-        <is>
-          <t>5th</t>
+          <t>Zach</t>
+        </is>
+      </c>
+      <c r="E8" s="14" t="n">
+        <v>15</v>
+      </c>
+      <c r="F8" s="14" t="inlineStr">
+        <is>
+          <t>DNP</t>
+        </is>
+      </c>
+      <c r="G8" s="16" t="inlineStr">
+        <is>
+          <t>3rd</t>
         </is>
       </c>
       <c r="H8" s="18" t="inlineStr">
         <is>
-          <t xml:space="preserve">Ray </t>
-        </is>
-      </c>
-      <c r="I8" s="19" t="n">
-        <v>12</v>
-      </c>
-      <c r="J8" s="19" t="inlineStr">
-        <is>
-          <t>4th</t>
-        </is>
-      </c>
-      <c r="K8" s="11" t="inlineStr">
-        <is>
-          <t>5th</t>
-        </is>
-      </c>
-      <c r="L8" s="10" t="inlineStr">
-        <is>
-          <t>4th</t>
+          <t>Zach</t>
+        </is>
+      </c>
+      <c r="I8" s="14" t="n">
+        <v>15</v>
+      </c>
+      <c r="J8" s="14" t="inlineStr">
+        <is>
+          <t>DNP</t>
+        </is>
+      </c>
+      <c r="K8" s="13" t="inlineStr">
+        <is>
+          <t>3rd</t>
+        </is>
+      </c>
+      <c r="L8" s="17" t="inlineStr">
+        <is>
+          <t>DNP</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="21" t="inlineStr">
+      <c r="A9" s="19" t="inlineStr">
         <is>
           <t>Steve</t>
         </is>
       </c>
-      <c r="B9" s="22" t="n">
+      <c r="B9" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="C9" s="23" t="inlineStr">
-        <is>
-          <t>DNP</t>
-        </is>
-      </c>
-      <c r="D9" s="21" t="inlineStr">
+      <c r="C9" s="21" t="inlineStr">
+        <is>
+          <t>DNP</t>
+        </is>
+      </c>
+      <c r="D9" s="19" t="inlineStr">
         <is>
           <t>Steve</t>
         </is>
       </c>
-      <c r="E9" s="22" t="n">
+      <c r="E9" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="F9" s="22" t="inlineStr">
-        <is>
-          <t>DNP</t>
-        </is>
-      </c>
-      <c r="G9" s="24" t="inlineStr">
-        <is>
-          <t>DNP</t>
-        </is>
-      </c>
-      <c r="H9" s="21" t="inlineStr">
+      <c r="F9" s="20" t="inlineStr">
+        <is>
+          <t>DNP</t>
+        </is>
+      </c>
+      <c r="G9" s="21" t="inlineStr">
+        <is>
+          <t>DNP</t>
+        </is>
+      </c>
+      <c r="H9" s="19" t="inlineStr">
         <is>
           <t>Steve</t>
         </is>
       </c>
-      <c r="I9" s="22" t="n">
+      <c r="I9" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="J9" s="22" t="inlineStr">
-        <is>
-          <t>DNP</t>
-        </is>
-      </c>
-      <c r="K9" s="25" t="inlineStr">
-        <is>
-          <t>DNP</t>
-        </is>
-      </c>
-      <c r="L9" s="24" t="inlineStr">
+      <c r="J9" s="20" t="inlineStr">
+        <is>
+          <t>DNP</t>
+        </is>
+      </c>
+      <c r="K9" s="20" t="inlineStr">
+        <is>
+          <t>DNP</t>
+        </is>
+      </c>
+      <c r="L9" s="21" t="inlineStr">
         <is>
           <t>DNP</t>
         </is>
@@ -1541,9 +1526,9 @@
         </is>
       </c>
       <c r="E4" s="8" t="n">
-        <v>25</v>
-      </c>
-      <c r="F4" s="11" t="inlineStr">
+        <v>43</v>
+      </c>
+      <c r="F4" s="12" t="inlineStr">
         <is>
           <t>2nd</t>
         </is>
@@ -1555,81 +1540,81 @@
       </c>
       <c r="H4" s="7" t="inlineStr">
         <is>
+          <t>Evan</t>
+        </is>
+      </c>
+      <c r="I4" s="8" t="n">
+        <v>61</v>
+      </c>
+      <c r="J4" s="12" t="inlineStr">
+        <is>
+          <t>2nd</t>
+        </is>
+      </c>
+      <c r="K4" s="8" t="inlineStr">
+        <is>
+          <t>1st</t>
+        </is>
+      </c>
+      <c r="L4" s="10" t="inlineStr">
+        <is>
+          <t>2nd</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="11" t="inlineStr">
+        <is>
+          <t>Evan</t>
+        </is>
+      </c>
+      <c r="B5" s="12" t="n">
+        <v>18</v>
+      </c>
+      <c r="C5" s="10" t="inlineStr">
+        <is>
+          <t>2nd</t>
+        </is>
+      </c>
+      <c r="D5" s="11" t="inlineStr">
+        <is>
           <t>Nathan</t>
         </is>
       </c>
-      <c r="I4" s="8" t="n">
-        <v>25</v>
-      </c>
-      <c r="J4" s="8" t="inlineStr">
+      <c r="E5" s="12" t="n">
+        <v>35</v>
+      </c>
+      <c r="F5" s="8" t="inlineStr">
         <is>
           <t>1st</t>
         </is>
       </c>
-      <c r="K4" s="11" t="inlineStr">
+      <c r="G5" s="17" t="inlineStr">
         <is>
           <t>5th</t>
         </is>
       </c>
-      <c r="L4" s="10" t="inlineStr">
+      <c r="H5" s="11" t="inlineStr">
+        <is>
+          <t>Nathan</t>
+        </is>
+      </c>
+      <c r="I5" s="12" t="n">
+        <v>60</v>
+      </c>
+      <c r="J5" s="8" t="inlineStr">
         <is>
           <t>1st</t>
         </is>
       </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="12" t="inlineStr">
-        <is>
-          <t>Evan</t>
-        </is>
-      </c>
-      <c r="B5" s="13" t="n">
-        <v>18</v>
-      </c>
-      <c r="C5" s="14" t="inlineStr">
-        <is>
-          <t>2nd</t>
-        </is>
-      </c>
-      <c r="D5" s="12" t="inlineStr">
-        <is>
-          <t>Nathan</t>
-        </is>
-      </c>
-      <c r="E5" s="13" t="n">
-        <v>25</v>
-      </c>
-      <c r="F5" s="8" t="inlineStr">
+      <c r="K5" s="14" t="inlineStr">
+        <is>
+          <t>5th</t>
+        </is>
+      </c>
+      <c r="L5" s="9" t="inlineStr">
         <is>
           <t>1st</t>
-        </is>
-      </c>
-      <c r="G5" s="10" t="inlineStr">
-        <is>
-          <t>5th</t>
-        </is>
-      </c>
-      <c r="H5" s="12" t="inlineStr">
-        <is>
-          <t>Evan</t>
-        </is>
-      </c>
-      <c r="I5" s="13" t="n">
-        <v>25</v>
-      </c>
-      <c r="J5" s="11" t="inlineStr">
-        <is>
-          <t>2nd</t>
-        </is>
-      </c>
-      <c r="K5" s="8" t="inlineStr">
-        <is>
-          <t>1st</t>
-        </is>
-      </c>
-      <c r="L5" s="10" t="inlineStr">
-        <is>
-          <t>2nd</t>
         </is>
       </c>
     </row>
@@ -1639,10 +1624,10 @@
           <t xml:space="preserve">Ray </t>
         </is>
       </c>
-      <c r="B6" s="16" t="n">
+      <c r="B6" s="13" t="n">
         <v>15</v>
       </c>
-      <c r="C6" s="17" t="inlineStr">
+      <c r="C6" s="16" t="inlineStr">
         <is>
           <t>3rd</t>
         </is>
@@ -1652,15 +1637,15 @@
           <t>Mike</t>
         </is>
       </c>
-      <c r="E6" s="16" t="n">
-        <v>18</v>
-      </c>
-      <c r="F6" s="11" t="inlineStr">
+      <c r="E6" s="13" t="n">
+        <v>30</v>
+      </c>
+      <c r="F6" s="14" t="inlineStr">
         <is>
           <t>4th</t>
         </is>
       </c>
-      <c r="G6" s="14" t="inlineStr">
+      <c r="G6" s="10" t="inlineStr">
         <is>
           <t>2nd</t>
         </is>
@@ -1670,20 +1655,20 @@
           <t>Mike</t>
         </is>
       </c>
-      <c r="I6" s="16" t="n">
-        <v>18</v>
-      </c>
-      <c r="J6" s="11" t="inlineStr">
+      <c r="I6" s="13" t="n">
+        <v>45</v>
+      </c>
+      <c r="J6" s="14" t="inlineStr">
         <is>
           <t>4th</t>
         </is>
       </c>
-      <c r="K6" s="13" t="inlineStr">
+      <c r="K6" s="12" t="inlineStr">
         <is>
           <t>2nd</t>
         </is>
       </c>
-      <c r="L6" s="10" t="inlineStr">
+      <c r="L6" s="16" t="inlineStr">
         <is>
           <t>3rd</t>
         </is>
@@ -1695,10 +1680,10 @@
           <t>Mike</t>
         </is>
       </c>
-      <c r="B7" s="19" t="n">
+      <c r="B7" s="14" t="n">
         <v>12</v>
       </c>
-      <c r="C7" s="20" t="inlineStr">
+      <c r="C7" s="17" t="inlineStr">
         <is>
           <t>4th</t>
         </is>
@@ -1708,15 +1693,15 @@
           <t xml:space="preserve">Ray </t>
         </is>
       </c>
-      <c r="E7" s="19" t="n">
-        <v>15</v>
-      </c>
-      <c r="F7" s="16" t="inlineStr">
+      <c r="E7" s="14" t="n">
+        <v>27</v>
+      </c>
+      <c r="F7" s="13" t="inlineStr">
         <is>
           <t>3rd</t>
         </is>
       </c>
-      <c r="G7" s="10" t="inlineStr">
+      <c r="G7" s="17" t="inlineStr">
         <is>
           <t>4th</t>
         </is>
@@ -1726,20 +1711,20 @@
           <t xml:space="preserve">Ray </t>
         </is>
       </c>
-      <c r="I7" s="19" t="n">
-        <v>15</v>
-      </c>
-      <c r="J7" s="16" t="inlineStr">
+      <c r="I7" s="14" t="n">
+        <v>39</v>
+      </c>
+      <c r="J7" s="13" t="inlineStr">
         <is>
           <t>3rd</t>
         </is>
       </c>
-      <c r="K7" s="11" t="inlineStr">
+      <c r="K7" s="14" t="inlineStr">
         <is>
           <t>4th</t>
         </is>
       </c>
-      <c r="L7" s="10" t="inlineStr">
+      <c r="L7" s="17" t="inlineStr">
         <is>
           <t>4th</t>
         </is>
@@ -1751,10 +1736,10 @@
           <t>Zach</t>
         </is>
       </c>
-      <c r="B8" s="19" t="n">
+      <c r="B8" s="14" t="n">
         <v>0</v>
       </c>
-      <c r="C8" s="20" t="inlineStr">
+      <c r="C8" s="17" t="inlineStr">
         <is>
           <t>DNP</t>
         </is>
@@ -1764,15 +1749,15 @@
           <t>Zach</t>
         </is>
       </c>
-      <c r="E8" s="19" t="n">
+      <c r="E8" s="14" t="n">
         <v>15</v>
       </c>
-      <c r="F8" s="11" t="inlineStr">
-        <is>
-          <t>DNP</t>
-        </is>
-      </c>
-      <c r="G8" s="17" t="inlineStr">
+      <c r="F8" s="14" t="inlineStr">
+        <is>
+          <t>DNP</t>
+        </is>
+      </c>
+      <c r="G8" s="16" t="inlineStr">
         <is>
           <t>3rd</t>
         </is>
@@ -1782,76 +1767,76 @@
           <t>Zach</t>
         </is>
       </c>
-      <c r="I8" s="19" t="n">
+      <c r="I8" s="14" t="n">
         <v>15</v>
       </c>
-      <c r="J8" s="11" t="inlineStr">
-        <is>
-          <t>DNP</t>
-        </is>
-      </c>
-      <c r="K8" s="16" t="inlineStr">
+      <c r="J8" s="14" t="inlineStr">
+        <is>
+          <t>DNP</t>
+        </is>
+      </c>
+      <c r="K8" s="13" t="inlineStr">
         <is>
           <t>3rd</t>
         </is>
       </c>
-      <c r="L8" s="10" t="inlineStr">
+      <c r="L8" s="17" t="inlineStr">
         <is>
           <t>DNP</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="21" t="inlineStr">
+      <c r="A9" s="19" t="inlineStr">
         <is>
           <t>Steve</t>
         </is>
       </c>
-      <c r="B9" s="22" t="n">
+      <c r="B9" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="C9" s="23" t="inlineStr">
-        <is>
-          <t>DNP</t>
-        </is>
-      </c>
-      <c r="D9" s="21" t="inlineStr">
+      <c r="C9" s="21" t="inlineStr">
+        <is>
+          <t>DNP</t>
+        </is>
+      </c>
+      <c r="D9" s="19" t="inlineStr">
         <is>
           <t>Steve</t>
         </is>
       </c>
-      <c r="E9" s="22" t="n">
+      <c r="E9" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="F9" s="22" t="inlineStr">
-        <is>
-          <t>DNP</t>
-        </is>
-      </c>
-      <c r="G9" s="24" t="inlineStr">
-        <is>
-          <t>DNP</t>
-        </is>
-      </c>
-      <c r="H9" s="21" t="inlineStr">
+      <c r="F9" s="20" t="inlineStr">
+        <is>
+          <t>DNP</t>
+        </is>
+      </c>
+      <c r="G9" s="21" t="inlineStr">
+        <is>
+          <t>DNP</t>
+        </is>
+      </c>
+      <c r="H9" s="19" t="inlineStr">
         <is>
           <t>Steve</t>
         </is>
       </c>
-      <c r="I9" s="22" t="n">
+      <c r="I9" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="J9" s="22" t="inlineStr">
-        <is>
-          <t>DNP</t>
-        </is>
-      </c>
-      <c r="K9" s="25" t="inlineStr">
-        <is>
-          <t>DNP</t>
-        </is>
-      </c>
-      <c r="L9" s="24" t="inlineStr">
+      <c r="J9" s="20" t="inlineStr">
+        <is>
+          <t>DNP</t>
+        </is>
+      </c>
+      <c r="K9" s="20" t="inlineStr">
+        <is>
+          <t>DNP</t>
+        </is>
+      </c>
+      <c r="L9" s="21" t="inlineStr">
         <is>
           <t>DNP</t>
         </is>

</xml_diff>

<commit_message>
Ran Pycharm auto code cleanup.
</commit_message>
<xml_diff>
--- a/out.xlsx
+++ b/out.xlsx
@@ -19,7 +19,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -45,6 +45,9 @@
     <font>
       <b val="1"/>
       <color rgb="00CD7F32"/>
+    </font>
+    <font>
+      <color rgb="00e6e6e6"/>
     </font>
   </fonts>
   <fills count="6">
@@ -195,7 +198,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -222,33 +225,39 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -256,6 +265,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1068,14 +1083,14 @@
         </is>
       </c>
       <c r="E4" s="8" t="n">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="F4" s="8" t="inlineStr">
         <is>
           <t>1st</t>
         </is>
       </c>
-      <c r="G4" s="9" t="inlineStr">
+      <c r="G4" s="10" t="inlineStr">
         <is>
           <t>1st</t>
         </is>
@@ -1086,14 +1101,14 @@
         </is>
       </c>
       <c r="I4" s="8" t="n">
-        <v>68</v>
+        <v>25</v>
       </c>
       <c r="J4" s="8" t="inlineStr">
         <is>
           <t>1st</t>
         </is>
       </c>
-      <c r="K4" s="8" t="inlineStr">
+      <c r="K4" s="11" t="inlineStr">
         <is>
           <t>1st</t>
         </is>
@@ -1105,28 +1120,28 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="11" t="inlineStr">
+      <c r="A5" s="12" t="inlineStr">
         <is>
           <t>Evan</t>
         </is>
       </c>
-      <c r="B5" s="12" t="n">
+      <c r="B5" s="13" t="n">
         <v>18</v>
       </c>
-      <c r="C5" s="10" t="inlineStr">
+      <c r="C5" s="14" t="inlineStr">
         <is>
           <t>2nd</t>
         </is>
       </c>
-      <c r="D5" s="11" t="inlineStr">
+      <c r="D5" s="12" t="inlineStr">
         <is>
           <t>Evan</t>
         </is>
       </c>
-      <c r="E5" s="12" t="n">
-        <v>36</v>
-      </c>
-      <c r="F5" s="12" t="inlineStr">
+      <c r="E5" s="13" t="n">
+        <v>18</v>
+      </c>
+      <c r="F5" s="13" t="inlineStr">
         <is>
           <t>2nd</t>
         </is>
@@ -1136,20 +1151,20 @@
           <t>2nd</t>
         </is>
       </c>
-      <c r="H5" s="11" t="inlineStr">
+      <c r="H5" s="12" t="inlineStr">
         <is>
           <t>Mike</t>
         </is>
       </c>
-      <c r="I5" s="12" t="n">
-        <v>52</v>
-      </c>
-      <c r="J5" s="13" t="inlineStr">
+      <c r="I5" s="13" t="n">
+        <v>25</v>
+      </c>
+      <c r="J5" s="11" t="inlineStr">
         <is>
           <t>3rd</t>
         </is>
       </c>
-      <c r="K5" s="14" t="inlineStr">
+      <c r="K5" s="11" t="inlineStr">
         <is>
           <t>4th</t>
         </is>
@@ -1166,10 +1181,10 @@
           <t>Mike</t>
         </is>
       </c>
-      <c r="B6" s="13" t="n">
+      <c r="B6" s="16" t="n">
         <v>15</v>
       </c>
-      <c r="C6" s="16" t="inlineStr">
+      <c r="C6" s="17" t="inlineStr">
         <is>
           <t>3rd</t>
         </is>
@@ -1179,15 +1194,15 @@
           <t>Mike</t>
         </is>
       </c>
-      <c r="E6" s="13" t="n">
-        <v>27</v>
-      </c>
-      <c r="F6" s="13" t="inlineStr">
+      <c r="E6" s="16" t="n">
+        <v>15</v>
+      </c>
+      <c r="F6" s="16" t="inlineStr">
         <is>
           <t>3rd</t>
         </is>
       </c>
-      <c r="G6" s="17" t="inlineStr">
+      <c r="G6" s="10" t="inlineStr">
         <is>
           <t>4th</t>
         </is>
@@ -1197,20 +1212,20 @@
           <t>Evan</t>
         </is>
       </c>
-      <c r="I6" s="13" t="n">
-        <v>51</v>
-      </c>
-      <c r="J6" s="12" t="inlineStr">
+      <c r="I6" s="16" t="n">
+        <v>18</v>
+      </c>
+      <c r="J6" s="13" t="inlineStr">
         <is>
           <t>2nd</t>
         </is>
       </c>
-      <c r="K6" s="12" t="inlineStr">
+      <c r="K6" s="11" t="inlineStr">
         <is>
           <t>2nd</t>
         </is>
       </c>
-      <c r="L6" s="16" t="inlineStr">
+      <c r="L6" s="10" t="inlineStr">
         <is>
           <t>3rd</t>
         </is>
@@ -1222,53 +1237,53 @@
           <t xml:space="preserve">Ray </t>
         </is>
       </c>
-      <c r="B7" s="14" t="n">
+      <c r="B7" s="19" t="n">
         <v>12</v>
       </c>
-      <c r="C7" s="17" t="inlineStr">
+      <c r="C7" s="20" t="inlineStr">
         <is>
           <t>4th</t>
         </is>
       </c>
       <c r="D7" s="18" t="inlineStr">
         <is>
-          <t xml:space="preserve">Ray </t>
-        </is>
-      </c>
-      <c r="E7" s="14" t="n">
-        <v>22</v>
-      </c>
-      <c r="F7" s="14" t="inlineStr">
-        <is>
-          <t>4th</t>
+          <t>Zach</t>
+        </is>
+      </c>
+      <c r="E7" s="19" t="n">
+        <v>15</v>
+      </c>
+      <c r="F7" s="11" t="inlineStr">
+        <is>
+          <t>DNP</t>
         </is>
       </c>
       <c r="G7" s="17" t="inlineStr">
         <is>
-          <t>5th</t>
+          <t>3rd</t>
         </is>
       </c>
       <c r="H7" s="18" t="inlineStr">
         <is>
-          <t xml:space="preserve">Ray </t>
-        </is>
-      </c>
-      <c r="I7" s="14" t="n">
-        <v>34</v>
-      </c>
-      <c r="J7" s="14" t="inlineStr">
-        <is>
-          <t>4th</t>
-        </is>
-      </c>
-      <c r="K7" s="14" t="inlineStr">
-        <is>
-          <t>5th</t>
-        </is>
-      </c>
-      <c r="L7" s="17" t="inlineStr">
-        <is>
-          <t>4th</t>
+          <t>Zach</t>
+        </is>
+      </c>
+      <c r="I7" s="19" t="n">
+        <v>15</v>
+      </c>
+      <c r="J7" s="11" t="inlineStr">
+        <is>
+          <t>DNP</t>
+        </is>
+      </c>
+      <c r="K7" s="16" t="inlineStr">
+        <is>
+          <t>3rd</t>
+        </is>
+      </c>
+      <c r="L7" s="10" t="inlineStr">
+        <is>
+          <t>DNP</t>
         </is>
       </c>
     </row>
@@ -1278,107 +1293,107 @@
           <t>Zach</t>
         </is>
       </c>
-      <c r="B8" s="14" t="n">
+      <c r="B8" s="19" t="n">
         <v>0</v>
       </c>
-      <c r="C8" s="17" t="inlineStr">
+      <c r="C8" s="20" t="inlineStr">
         <is>
           <t>DNP</t>
         </is>
       </c>
       <c r="D8" s="18" t="inlineStr">
         <is>
-          <t>Zach</t>
-        </is>
-      </c>
-      <c r="E8" s="14" t="n">
-        <v>15</v>
-      </c>
-      <c r="F8" s="14" t="inlineStr">
-        <is>
-          <t>DNP</t>
-        </is>
-      </c>
-      <c r="G8" s="16" t="inlineStr">
-        <is>
-          <t>3rd</t>
+          <t xml:space="preserve">Ray </t>
+        </is>
+      </c>
+      <c r="E8" s="19" t="n">
+        <v>12</v>
+      </c>
+      <c r="F8" s="19" t="inlineStr">
+        <is>
+          <t>4th</t>
+        </is>
+      </c>
+      <c r="G8" s="10" t="inlineStr">
+        <is>
+          <t>5th</t>
         </is>
       </c>
       <c r="H8" s="18" t="inlineStr">
         <is>
-          <t>Zach</t>
-        </is>
-      </c>
-      <c r="I8" s="14" t="n">
-        <v>15</v>
-      </c>
-      <c r="J8" s="14" t="inlineStr">
-        <is>
-          <t>DNP</t>
-        </is>
-      </c>
-      <c r="K8" s="13" t="inlineStr">
-        <is>
-          <t>3rd</t>
-        </is>
-      </c>
-      <c r="L8" s="17" t="inlineStr">
-        <is>
-          <t>DNP</t>
+          <t xml:space="preserve">Ray </t>
+        </is>
+      </c>
+      <c r="I8" s="19" t="n">
+        <v>12</v>
+      </c>
+      <c r="J8" s="19" t="inlineStr">
+        <is>
+          <t>4th</t>
+        </is>
+      </c>
+      <c r="K8" s="11" t="inlineStr">
+        <is>
+          <t>5th</t>
+        </is>
+      </c>
+      <c r="L8" s="10" t="inlineStr">
+        <is>
+          <t>4th</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="19" t="inlineStr">
+      <c r="A9" s="21" t="inlineStr">
         <is>
           <t>Steve</t>
         </is>
       </c>
-      <c r="B9" s="20" t="n">
+      <c r="B9" s="22" t="n">
         <v>0</v>
       </c>
-      <c r="C9" s="21" t="inlineStr">
-        <is>
-          <t>DNP</t>
-        </is>
-      </c>
-      <c r="D9" s="19" t="inlineStr">
+      <c r="C9" s="23" t="inlineStr">
+        <is>
+          <t>DNP</t>
+        </is>
+      </c>
+      <c r="D9" s="21" t="inlineStr">
         <is>
           <t>Steve</t>
         </is>
       </c>
-      <c r="E9" s="20" t="n">
+      <c r="E9" s="22" t="n">
         <v>0</v>
       </c>
-      <c r="F9" s="20" t="inlineStr">
-        <is>
-          <t>DNP</t>
-        </is>
-      </c>
-      <c r="G9" s="21" t="inlineStr">
-        <is>
-          <t>DNP</t>
-        </is>
-      </c>
-      <c r="H9" s="19" t="inlineStr">
+      <c r="F9" s="22" t="inlineStr">
+        <is>
+          <t>DNP</t>
+        </is>
+      </c>
+      <c r="G9" s="24" t="inlineStr">
+        <is>
+          <t>DNP</t>
+        </is>
+      </c>
+      <c r="H9" s="21" t="inlineStr">
         <is>
           <t>Steve</t>
         </is>
       </c>
-      <c r="I9" s="20" t="n">
+      <c r="I9" s="22" t="n">
         <v>0</v>
       </c>
-      <c r="J9" s="20" t="inlineStr">
-        <is>
-          <t>DNP</t>
-        </is>
-      </c>
-      <c r="K9" s="20" t="inlineStr">
-        <is>
-          <t>DNP</t>
-        </is>
-      </c>
-      <c r="L9" s="21" t="inlineStr">
+      <c r="J9" s="22" t="inlineStr">
+        <is>
+          <t>DNP</t>
+        </is>
+      </c>
+      <c r="K9" s="25" t="inlineStr">
+        <is>
+          <t>DNP</t>
+        </is>
+      </c>
+      <c r="L9" s="24" t="inlineStr">
         <is>
           <t>DNP</t>
         </is>
@@ -1526,9 +1541,9 @@
         </is>
       </c>
       <c r="E4" s="8" t="n">
-        <v>43</v>
-      </c>
-      <c r="F4" s="12" t="inlineStr">
+        <v>25</v>
+      </c>
+      <c r="F4" s="11" t="inlineStr">
         <is>
           <t>2nd</t>
         </is>
@@ -1540,81 +1555,81 @@
       </c>
       <c r="H4" s="7" t="inlineStr">
         <is>
+          <t>Nathan</t>
+        </is>
+      </c>
+      <c r="I4" s="8" t="n">
+        <v>25</v>
+      </c>
+      <c r="J4" s="8" t="inlineStr">
+        <is>
+          <t>1st</t>
+        </is>
+      </c>
+      <c r="K4" s="11" t="inlineStr">
+        <is>
+          <t>5th</t>
+        </is>
+      </c>
+      <c r="L4" s="10" t="inlineStr">
+        <is>
+          <t>1st</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="12" t="inlineStr">
+        <is>
           <t>Evan</t>
         </is>
       </c>
-      <c r="I4" s="8" t="n">
-        <v>61</v>
-      </c>
-      <c r="J4" s="12" t="inlineStr">
+      <c r="B5" s="13" t="n">
+        <v>18</v>
+      </c>
+      <c r="C5" s="14" t="inlineStr">
         <is>
           <t>2nd</t>
         </is>
       </c>
-      <c r="K4" s="8" t="inlineStr">
+      <c r="D5" s="12" t="inlineStr">
+        <is>
+          <t>Nathan</t>
+        </is>
+      </c>
+      <c r="E5" s="13" t="n">
+        <v>25</v>
+      </c>
+      <c r="F5" s="8" t="inlineStr">
         <is>
           <t>1st</t>
         </is>
       </c>
-      <c r="L4" s="10" t="inlineStr">
+      <c r="G5" s="10" t="inlineStr">
+        <is>
+          <t>5th</t>
+        </is>
+      </c>
+      <c r="H5" s="12" t="inlineStr">
+        <is>
+          <t>Evan</t>
+        </is>
+      </c>
+      <c r="I5" s="13" t="n">
+        <v>25</v>
+      </c>
+      <c r="J5" s="11" t="inlineStr">
         <is>
           <t>2nd</t>
         </is>
       </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="11" t="inlineStr">
-        <is>
-          <t>Evan</t>
-        </is>
-      </c>
-      <c r="B5" s="12" t="n">
-        <v>18</v>
-      </c>
-      <c r="C5" s="10" t="inlineStr">
+      <c r="K5" s="8" t="inlineStr">
+        <is>
+          <t>1st</t>
+        </is>
+      </c>
+      <c r="L5" s="10" t="inlineStr">
         <is>
           <t>2nd</t>
-        </is>
-      </c>
-      <c r="D5" s="11" t="inlineStr">
-        <is>
-          <t>Nathan</t>
-        </is>
-      </c>
-      <c r="E5" s="12" t="n">
-        <v>35</v>
-      </c>
-      <c r="F5" s="8" t="inlineStr">
-        <is>
-          <t>1st</t>
-        </is>
-      </c>
-      <c r="G5" s="17" t="inlineStr">
-        <is>
-          <t>5th</t>
-        </is>
-      </c>
-      <c r="H5" s="11" t="inlineStr">
-        <is>
-          <t>Nathan</t>
-        </is>
-      </c>
-      <c r="I5" s="12" t="n">
-        <v>60</v>
-      </c>
-      <c r="J5" s="8" t="inlineStr">
-        <is>
-          <t>1st</t>
-        </is>
-      </c>
-      <c r="K5" s="14" t="inlineStr">
-        <is>
-          <t>5th</t>
-        </is>
-      </c>
-      <c r="L5" s="9" t="inlineStr">
-        <is>
-          <t>1st</t>
         </is>
       </c>
     </row>
@@ -1624,10 +1639,10 @@
           <t xml:space="preserve">Ray </t>
         </is>
       </c>
-      <c r="B6" s="13" t="n">
+      <c r="B6" s="16" t="n">
         <v>15</v>
       </c>
-      <c r="C6" s="16" t="inlineStr">
+      <c r="C6" s="17" t="inlineStr">
         <is>
           <t>3rd</t>
         </is>
@@ -1637,15 +1652,15 @@
           <t>Mike</t>
         </is>
       </c>
-      <c r="E6" s="13" t="n">
-        <v>30</v>
-      </c>
-      <c r="F6" s="14" t="inlineStr">
+      <c r="E6" s="16" t="n">
+        <v>18</v>
+      </c>
+      <c r="F6" s="11" t="inlineStr">
         <is>
           <t>4th</t>
         </is>
       </c>
-      <c r="G6" s="10" t="inlineStr">
+      <c r="G6" s="14" t="inlineStr">
         <is>
           <t>2nd</t>
         </is>
@@ -1655,20 +1670,20 @@
           <t>Mike</t>
         </is>
       </c>
-      <c r="I6" s="13" t="n">
-        <v>45</v>
-      </c>
-      <c r="J6" s="14" t="inlineStr">
+      <c r="I6" s="16" t="n">
+        <v>18</v>
+      </c>
+      <c r="J6" s="11" t="inlineStr">
         <is>
           <t>4th</t>
         </is>
       </c>
-      <c r="K6" s="12" t="inlineStr">
+      <c r="K6" s="13" t="inlineStr">
         <is>
           <t>2nd</t>
         </is>
       </c>
-      <c r="L6" s="16" t="inlineStr">
+      <c r="L6" s="10" t="inlineStr">
         <is>
           <t>3rd</t>
         </is>
@@ -1680,10 +1695,10 @@
           <t>Mike</t>
         </is>
       </c>
-      <c r="B7" s="14" t="n">
+      <c r="B7" s="19" t="n">
         <v>12</v>
       </c>
-      <c r="C7" s="17" t="inlineStr">
+      <c r="C7" s="20" t="inlineStr">
         <is>
           <t>4th</t>
         </is>
@@ -1693,15 +1708,15 @@
           <t xml:space="preserve">Ray </t>
         </is>
       </c>
-      <c r="E7" s="14" t="n">
-        <v>27</v>
-      </c>
-      <c r="F7" s="13" t="inlineStr">
+      <c r="E7" s="19" t="n">
+        <v>15</v>
+      </c>
+      <c r="F7" s="16" t="inlineStr">
         <is>
           <t>3rd</t>
         </is>
       </c>
-      <c r="G7" s="17" t="inlineStr">
+      <c r="G7" s="10" t="inlineStr">
         <is>
           <t>4th</t>
         </is>
@@ -1711,20 +1726,20 @@
           <t xml:space="preserve">Ray </t>
         </is>
       </c>
-      <c r="I7" s="14" t="n">
-        <v>39</v>
-      </c>
-      <c r="J7" s="13" t="inlineStr">
+      <c r="I7" s="19" t="n">
+        <v>15</v>
+      </c>
+      <c r="J7" s="16" t="inlineStr">
         <is>
           <t>3rd</t>
         </is>
       </c>
-      <c r="K7" s="14" t="inlineStr">
+      <c r="K7" s="11" t="inlineStr">
         <is>
           <t>4th</t>
         </is>
       </c>
-      <c r="L7" s="17" t="inlineStr">
+      <c r="L7" s="10" t="inlineStr">
         <is>
           <t>4th</t>
         </is>
@@ -1736,10 +1751,10 @@
           <t>Zach</t>
         </is>
       </c>
-      <c r="B8" s="14" t="n">
+      <c r="B8" s="19" t="n">
         <v>0</v>
       </c>
-      <c r="C8" s="17" t="inlineStr">
+      <c r="C8" s="20" t="inlineStr">
         <is>
           <t>DNP</t>
         </is>
@@ -1749,15 +1764,15 @@
           <t>Zach</t>
         </is>
       </c>
-      <c r="E8" s="14" t="n">
+      <c r="E8" s="19" t="n">
         <v>15</v>
       </c>
-      <c r="F8" s="14" t="inlineStr">
-        <is>
-          <t>DNP</t>
-        </is>
-      </c>
-      <c r="G8" s="16" t="inlineStr">
+      <c r="F8" s="11" t="inlineStr">
+        <is>
+          <t>DNP</t>
+        </is>
+      </c>
+      <c r="G8" s="17" t="inlineStr">
         <is>
           <t>3rd</t>
         </is>
@@ -1767,76 +1782,76 @@
           <t>Zach</t>
         </is>
       </c>
-      <c r="I8" s="14" t="n">
+      <c r="I8" s="19" t="n">
         <v>15</v>
       </c>
-      <c r="J8" s="14" t="inlineStr">
-        <is>
-          <t>DNP</t>
-        </is>
-      </c>
-      <c r="K8" s="13" t="inlineStr">
+      <c r="J8" s="11" t="inlineStr">
+        <is>
+          <t>DNP</t>
+        </is>
+      </c>
+      <c r="K8" s="16" t="inlineStr">
         <is>
           <t>3rd</t>
         </is>
       </c>
-      <c r="L8" s="17" t="inlineStr">
+      <c r="L8" s="10" t="inlineStr">
         <is>
           <t>DNP</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="19" t="inlineStr">
+      <c r="A9" s="21" t="inlineStr">
         <is>
           <t>Steve</t>
         </is>
       </c>
-      <c r="B9" s="20" t="n">
+      <c r="B9" s="22" t="n">
         <v>0</v>
       </c>
-      <c r="C9" s="21" t="inlineStr">
-        <is>
-          <t>DNP</t>
-        </is>
-      </c>
-      <c r="D9" s="19" t="inlineStr">
+      <c r="C9" s="23" t="inlineStr">
+        <is>
+          <t>DNP</t>
+        </is>
+      </c>
+      <c r="D9" s="21" t="inlineStr">
         <is>
           <t>Steve</t>
         </is>
       </c>
-      <c r="E9" s="20" t="n">
+      <c r="E9" s="22" t="n">
         <v>0</v>
       </c>
-      <c r="F9" s="20" t="inlineStr">
-        <is>
-          <t>DNP</t>
-        </is>
-      </c>
-      <c r="G9" s="21" t="inlineStr">
-        <is>
-          <t>DNP</t>
-        </is>
-      </c>
-      <c r="H9" s="19" t="inlineStr">
+      <c r="F9" s="22" t="inlineStr">
+        <is>
+          <t>DNP</t>
+        </is>
+      </c>
+      <c r="G9" s="24" t="inlineStr">
+        <is>
+          <t>DNP</t>
+        </is>
+      </c>
+      <c r="H9" s="21" t="inlineStr">
         <is>
           <t>Steve</t>
         </is>
       </c>
-      <c r="I9" s="20" t="n">
+      <c r="I9" s="22" t="n">
         <v>0</v>
       </c>
-      <c r="J9" s="20" t="inlineStr">
-        <is>
-          <t>DNP</t>
-        </is>
-      </c>
-      <c r="K9" s="20" t="inlineStr">
-        <is>
-          <t>DNP</t>
-        </is>
-      </c>
-      <c r="L9" s="21" t="inlineStr">
+      <c r="J9" s="22" t="inlineStr">
+        <is>
+          <t>DNP</t>
+        </is>
+      </c>
+      <c r="K9" s="25" t="inlineStr">
+        <is>
+          <t>DNP</t>
+        </is>
+      </c>
+      <c r="L9" s="24" t="inlineStr">
         <is>
           <t>DNP</t>
         </is>

</xml_diff>